<commit_message>
started updating gantt chart, fixed software schedule
</commit_message>
<xml_diff>
--- a/Admin stuff/ganttChart copy.xlsx
+++ b/Admin stuff/ganttChart copy.xlsx
@@ -1,17 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-33540" yWindow="-4660" windowWidth="24720" windowHeight="15460" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
-    <sheet name="GanttChart" sheetId="2" r:id="rId3"/>
+    <sheet name="GanttChart" sheetId="2" r:id="rId2"/>
+    <sheet name="original" sheetId="3" r:id="rId3"/>
+    <sheet name="oh shit" sheetId="4" r:id="rId4"/>
+    <sheet name="revised" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="80">
   <si>
     <t>Task</t>
   </si>
@@ -113,42 +115,6 @@
     <t>DC-AC Inverter BB &amp; Test</t>
   </si>
   <si>
-    <t>Week 1</t>
-  </si>
-  <si>
-    <t>Week 2</t>
-  </si>
-  <si>
-    <t>Week 3</t>
-  </si>
-  <si>
-    <t>Week 4</t>
-  </si>
-  <si>
-    <t>Week 5</t>
-  </si>
-  <si>
-    <t>Week 6</t>
-  </si>
-  <si>
-    <t>Week 7</t>
-  </si>
-  <si>
-    <t>Week 8</t>
-  </si>
-  <si>
-    <t>Week 9</t>
-  </si>
-  <si>
-    <t>Week 10</t>
-  </si>
-  <si>
-    <t>Week 11</t>
-  </si>
-  <si>
-    <t>Week 12</t>
-  </si>
-  <si>
     <t>week1</t>
   </si>
   <si>
@@ -239,10 +205,76 @@
     <t>Order Basic Parts, Lights</t>
   </si>
   <si>
-    <t>Hardware Group</t>
-  </si>
-  <si>
     <t>Test PCB</t>
+  </si>
+  <si>
+    <t>Hardware Group (Ryan, Felix, Jake)</t>
+  </si>
+  <si>
+    <t>Complete</t>
+  </si>
+  <si>
+    <t>Auxilary Drivers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Falimiarize with the CC3200 </t>
+  </si>
+  <si>
+    <t>Start Date</t>
+  </si>
+  <si>
+    <t>End Date</t>
+  </si>
+  <si>
+    <t>2 weeks</t>
+  </si>
+  <si>
+    <t>Duration 
+(in weeks)</t>
+  </si>
+  <si>
+    <t>Week 4
+2/9</t>
+  </si>
+  <si>
+    <t>Week 3
+2/2</t>
+  </si>
+  <si>
+    <t>Week 5
+2/16</t>
+  </si>
+  <si>
+    <t>Week 6
+2/23</t>
+  </si>
+  <si>
+    <t>Week 7
+3/2</t>
+  </si>
+  <si>
+    <t>Week 8
+3/9</t>
+  </si>
+  <si>
+    <t>Week 9
+3/16</t>
+  </si>
+  <si>
+    <t>Week 10
+3/23</t>
+  </si>
+  <si>
+    <t>Week 11
+3/30</t>
+  </si>
+  <si>
+    <t>Week 12
+4/6</t>
+  </si>
+  <si>
+    <t>Week 13
+4/13</t>
   </si>
 </sst>
 </file>
@@ -252,7 +284,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d;@"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -287,6 +319,13 @@
       <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -401,12 +440,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="-0.249977111117893"/>
+        <fgColor theme="3" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="46">
     <border>
       <left/>
       <right/>
@@ -483,9 +522,102 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right/>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
       <bottom style="medium">
         <color auto="1"/>
       </bottom>
@@ -496,7 +628,78 @@
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top style="thin">
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
         <color auto="1"/>
       </top>
       <bottom/>
@@ -506,10 +709,36 @@
       <left style="thin">
         <color auto="1"/>
       </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top style="thin">
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
         <color auto="1"/>
       </top>
       <bottom/>
@@ -519,12 +748,243 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right style="thin">
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
         <color auto="1"/>
       </right>
       <top/>
-      <bottom style="thin">
-        <color auto="1"/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="thick">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FFFF0000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -538,39 +998,22 @@
       <top style="medium">
         <color auto="1"/>
       </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color auto="1"/>
       </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
+      <right/>
       <top style="medium">
         <color auto="1"/>
       </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
       <bottom/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -578,8 +1021,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="132">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -594,45 +1043,97 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="18" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="16" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="16" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="5" fillId="14" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="14" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="13" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="18" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -642,24 +1143,68 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="38" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="39" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="44" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -780,58 +1325,58 @@
                 <c:formatCode>m/d;@</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>41659</c:v>
+                  <c:v>41659.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41673</c:v>
+                  <c:v>41673.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>41673</c:v>
+                  <c:v>41673.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>41687</c:v>
+                  <c:v>41687.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>41687</c:v>
+                  <c:v>41687.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>41694</c:v>
+                  <c:v>41694.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>41687</c:v>
+                  <c:v>41687.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>41694</c:v>
+                  <c:v>41694.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>41715</c:v>
+                  <c:v>41715.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>41659</c:v>
+                  <c:v>41659.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>41666</c:v>
+                  <c:v>41666.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>41659</c:v>
+                  <c:v>41659.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>41687</c:v>
+                  <c:v>41687.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>41701</c:v>
+                  <c:v>41701.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>41659</c:v>
+                  <c:v>41659.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>41680</c:v>
+                  <c:v>41680.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>41694</c:v>
+                  <c:v>41694.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>41708</c:v>
+                  <c:v>41708.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -921,58 +1466,58 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -988,11 +1533,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="146565376"/>
-        <c:axId val="146567168"/>
+        <c:axId val="2107697992"/>
+        <c:axId val="2107701016"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="146565376"/>
+        <c:axId val="2107697992"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1002,7 +1547,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="146567168"/>
+        <c:crossAx val="2107701016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1010,11 +1555,11 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="146567168"/>
+        <c:axId val="2107701016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="41725"/>
-          <c:min val="41655"/>
+          <c:max val="41725.0"/>
+          <c:min val="41655.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="t"/>
@@ -1023,14 +1568,15 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="146565376"/>
+        <c:crossAx val="2107697992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="5"/>
+        <c:majorUnit val="5.0"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1044,7 +1590,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="116" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="115" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
@@ -1055,7 +1601,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8561552" cy="5824483"/>
+    <xdr:ext cx="8558696" cy="5819913"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -1406,20 +1952,20 @@
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="24.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.625" customWidth="1"/>
-    <col min="9" max="9" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.6640625" customWidth="1"/>
+    <col min="9" max="9" width="16.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" s="10" customFormat="1">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -1446,7 +1992,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" s="10" customFormat="1">
       <c r="A4" s="6" t="s">
         <v>17</v>
       </c>
@@ -1454,7 +2000,7 @@
         <v>41659</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="6">
@@ -1470,7 +2016,7 @@
       </c>
       <c r="I4" s="6"/>
     </row>
-    <row r="5" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" s="10" customFormat="1">
       <c r="A5" s="6" t="s">
         <v>29</v>
       </c>
@@ -1479,7 +2025,7 @@
         <v>41673</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="6">
@@ -1498,7 +2044,7 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" s="10" customFormat="1">
       <c r="A6" s="6" t="s">
         <v>6</v>
       </c>
@@ -1506,7 +2052,7 @@
         <v>41673</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="6">
@@ -1522,7 +2068,7 @@
       </c>
       <c r="I6" s="6"/>
     </row>
-    <row r="7" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" s="10" customFormat="1">
       <c r="A7" s="6" t="s">
         <v>28</v>
       </c>
@@ -1531,7 +2077,7 @@
         <v>41687</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="6">
@@ -1547,7 +2093,7 @@
       </c>
       <c r="I7" s="6"/>
     </row>
-    <row r="8" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" s="10" customFormat="1">
       <c r="A8" s="6" t="s">
         <v>9</v>
       </c>
@@ -1555,7 +2101,7 @@
         <v>41687</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="6">
@@ -1569,7 +2115,7 @@
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
     </row>
-    <row r="9" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" s="10" customFormat="1">
       <c r="A9" s="6" t="s">
         <v>27</v>
       </c>
@@ -1578,7 +2124,7 @@
         <v>41694</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="6">
@@ -1594,7 +2140,7 @@
       </c>
       <c r="I9" s="6"/>
     </row>
-    <row r="10" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" s="10" customFormat="1">
       <c r="A10" s="6" t="s">
         <v>26</v>
       </c>
@@ -1602,7 +2148,7 @@
         <v>41687</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="6">
@@ -1616,7 +2162,7 @@
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
     </row>
-    <row r="11" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" s="10" customFormat="1">
       <c r="A11" s="6" t="s">
         <v>25</v>
       </c>
@@ -1624,7 +2170,7 @@
         <v>41694</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="6">
@@ -1640,7 +2186,7 @@
       </c>
       <c r="I11" s="6"/>
     </row>
-    <row r="12" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" s="10" customFormat="1">
       <c r="A12" s="6" t="s">
         <v>19</v>
       </c>
@@ -1649,7 +2195,7 @@
         <v>41715</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="6">
@@ -1663,7 +2209,7 @@
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
     </row>
-    <row r="13" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" s="10" customFormat="1">
       <c r="A13" s="4" t="s">
         <v>14</v>
       </c>
@@ -1671,7 +2217,7 @@
         <v>41659</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="4">
@@ -1685,7 +2231,7 @@
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
     </row>
-    <row r="14" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" s="10" customFormat="1">
       <c r="A14" s="4" t="s">
         <v>12</v>
       </c>
@@ -1693,7 +2239,7 @@
         <v>41666</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" s="4">
@@ -1707,7 +2253,7 @@
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
     </row>
-    <row r="15" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" s="10" customFormat="1">
       <c r="A15" s="4" t="s">
         <v>13</v>
       </c>
@@ -1715,7 +2261,7 @@
         <v>41659</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="4">
@@ -1729,7 +2275,7 @@
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
     </row>
-    <row r="16" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" s="10" customFormat="1">
       <c r="A16" s="4" t="s">
         <v>15</v>
       </c>
@@ -1737,7 +2283,7 @@
         <v>41687</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="4">
@@ -1751,7 +2297,7 @@
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
     </row>
-    <row r="17" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" s="10" customFormat="1">
       <c r="A17" s="4" t="s">
         <v>16</v>
       </c>
@@ -1759,7 +2305,7 @@
         <v>41701</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="4">
@@ -1773,7 +2319,7 @@
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
     </row>
-    <row r="18" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" s="10" customFormat="1">
       <c r="A18" s="8" t="s">
         <v>21</v>
       </c>
@@ -1781,7 +2327,7 @@
         <v>41659</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="D18" s="9"/>
       <c r="E18" s="8">
@@ -1795,7 +2341,7 @@
       <c r="H18" s="8"/>
       <c r="I18" s="8"/>
     </row>
-    <row r="19" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" s="10" customFormat="1">
       <c r="A19" s="8" t="s">
         <v>22</v>
       </c>
@@ -1803,7 +2349,7 @@
         <v>41680</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="D19" s="9"/>
       <c r="E19" s="8">
@@ -1817,7 +2363,7 @@
       <c r="H19" s="8"/>
       <c r="I19" s="8"/>
     </row>
-    <row r="20" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" s="10" customFormat="1">
       <c r="A20" s="8" t="s">
         <v>23</v>
       </c>
@@ -1825,7 +2371,7 @@
         <v>41694</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="D20" s="9"/>
       <c r="E20" s="8">
@@ -1839,7 +2385,7 @@
       <c r="H20" s="8"/>
       <c r="I20" s="8"/>
     </row>
-    <row r="21" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" s="10" customFormat="1">
       <c r="A21" s="8" t="s">
         <v>24</v>
       </c>
@@ -1847,7 +2393,7 @@
         <v>41708</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="D21" s="9"/>
       <c r="E21" s="8">
@@ -1875,495 +2421,734 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M30"/>
+  <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView zoomScale="104" zoomScaleNormal="104" zoomScalePageLayoutView="104" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="26.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="13" width="9.625" customWidth="1"/>
+    <col min="1" max="1" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" customWidth="1"/>
+    <col min="3" max="3" width="9.5" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" customWidth="1"/>
+    <col min="5" max="14" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:14" ht="31" thickBot="1">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="C1" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="F1" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="G1" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="H1" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="I1" s="16" t="s">
+      <c r="B1" s="73" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="73" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="73" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" s="95" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" s="95" t="s">
+        <v>69</v>
+      </c>
+      <c r="G1" s="95" t="s">
+        <v>71</v>
+      </c>
+      <c r="H1" s="95" t="s">
+        <v>72</v>
+      </c>
+      <c r="I1" s="88" t="s">
+        <v>73</v>
+      </c>
+      <c r="J1" s="88" t="s">
+        <v>74</v>
+      </c>
+      <c r="K1" s="88" t="s">
+        <v>75</v>
+      </c>
+      <c r="L1" s="88" t="s">
+        <v>76</v>
+      </c>
+      <c r="M1" s="88" t="s">
+        <v>77</v>
+      </c>
+      <c r="N1" s="88" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="17" thickTop="1" thickBot="1">
+      <c r="A2" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="67">
+        <v>41672</v>
+      </c>
+      <c r="C2" s="74">
+        <v>1</v>
+      </c>
+      <c r="D2" s="67">
+        <f>B2+C2*7</f>
+        <v>41679</v>
+      </c>
+      <c r="E2" s="96"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="99"/>
+      <c r="I2" s="89"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="15"/>
+    </row>
+    <row r="3" spans="1:14" ht="16" thickBot="1">
+      <c r="A3" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="68">
+        <v>41672</v>
+      </c>
+      <c r="C3" s="75">
+        <v>2</v>
+      </c>
+      <c r="D3" s="68">
+        <f t="shared" ref="D3:D25" si="0">B3+C3*7</f>
+        <v>41686</v>
+      </c>
+      <c r="E3" s="100"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="101"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="30"/>
+      <c r="N3" s="15"/>
+    </row>
+    <row r="4" spans="1:14" ht="16" thickBot="1">
+      <c r="A4" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="68">
+        <v>41679</v>
+      </c>
+      <c r="C4" s="75">
+        <v>2</v>
+      </c>
+      <c r="D4" s="68">
+        <f t="shared" si="0"/>
+        <v>41693</v>
+      </c>
+      <c r="E4" s="102"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="50"/>
+      <c r="H4" s="101"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="30"/>
+      <c r="N4" s="15"/>
+    </row>
+    <row r="5" spans="1:14" ht="16" thickBot="1">
+      <c r="A5" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" s="68">
+        <v>41672</v>
+      </c>
+      <c r="C5" s="75">
+        <v>2</v>
+      </c>
+      <c r="D5" s="68">
+        <f t="shared" si="0"/>
+        <v>41686</v>
+      </c>
+      <c r="E5" s="103"/>
+      <c r="F5" s="51"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="101"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="30"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="30"/>
+      <c r="N5" s="15"/>
+    </row>
+    <row r="6" spans="1:14" ht="16" thickBot="1">
+      <c r="A6" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" s="68">
+        <v>41686</v>
+      </c>
+      <c r="C6" s="75">
+        <v>1</v>
+      </c>
+      <c r="D6" s="68">
+        <f t="shared" si="0"/>
+        <v>41693</v>
+      </c>
+      <c r="E6" s="104"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="52"/>
+      <c r="H6" s="101"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="30"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="30"/>
+      <c r="N6" s="15"/>
+    </row>
+    <row r="7" spans="1:14" ht="16" thickBot="1">
+      <c r="A7" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" s="68">
+        <v>41693</v>
+      </c>
+      <c r="C7" s="75">
+        <v>2</v>
+      </c>
+      <c r="D7" s="68">
+        <f t="shared" si="0"/>
+        <v>41707</v>
+      </c>
+      <c r="E7" s="104"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="41"/>
+      <c r="H7" s="105"/>
+      <c r="I7" s="48"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="30"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="30"/>
+      <c r="N7" s="15"/>
+    </row>
+    <row r="8" spans="1:14" ht="16" thickBot="1">
+      <c r="A8" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" s="68">
+        <v>41686</v>
+      </c>
+      <c r="C8" s="75">
+        <v>2</v>
+      </c>
+      <c r="D8" s="68">
+        <f t="shared" si="0"/>
+        <v>41700</v>
+      </c>
+      <c r="E8" s="104"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="81"/>
+      <c r="H8" s="106"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="30"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="30"/>
+      <c r="N8" s="15"/>
+    </row>
+    <row r="9" spans="1:14" ht="16" thickBot="1">
+      <c r="A9" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="68">
+        <v>41686</v>
+      </c>
+      <c r="C9" s="75">
+        <v>3</v>
+      </c>
+      <c r="D9" s="68">
+        <f t="shared" si="0"/>
+        <v>41707</v>
+      </c>
+      <c r="E9" s="104"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="49"/>
+      <c r="H9" s="107"/>
+      <c r="I9" s="48"/>
+      <c r="K9" s="30"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="30"/>
+      <c r="N9" s="15"/>
+    </row>
+    <row r="10" spans="1:14" ht="16" thickBot="1">
+      <c r="A10" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="68">
+        <v>41707</v>
+      </c>
+      <c r="C10" s="75">
+        <v>1</v>
+      </c>
+      <c r="D10" s="68">
+        <f t="shared" si="0"/>
+        <v>41714</v>
+      </c>
+      <c r="E10" s="104"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="101"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="53"/>
+      <c r="L10" s="30"/>
+      <c r="M10" s="30"/>
+      <c r="N10" s="15"/>
+    </row>
+    <row r="11" spans="1:14" ht="16" thickBot="1">
+      <c r="A11" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" s="68">
+        <v>41707</v>
+      </c>
+      <c r="C11" s="75">
+        <v>2</v>
+      </c>
+      <c r="D11" s="68">
+        <f t="shared" si="0"/>
+        <v>41721</v>
+      </c>
+      <c r="E11" s="104"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="101"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="81"/>
+      <c r="K11" s="48"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="30"/>
+      <c r="N11" s="15"/>
+    </row>
+    <row r="12" spans="1:14" ht="16" hidden="1" thickBot="1">
+      <c r="A12" s="64" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="69"/>
+      <c r="C12" s="76" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" s="67" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E12" s="108"/>
+      <c r="F12" s="54"/>
+      <c r="G12" s="30"/>
+      <c r="H12" s="101"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="30"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="30"/>
+      <c r="N12" s="15"/>
+    </row>
+    <row r="13" spans="1:14" ht="16" thickBot="1">
+      <c r="A13" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" s="70">
+        <v>41673</v>
+      </c>
+      <c r="C13" s="77">
+        <v>2</v>
+      </c>
+      <c r="D13" s="70">
+        <f t="shared" si="0"/>
+        <v>41687</v>
+      </c>
+      <c r="E13" s="109"/>
+      <c r="F13" s="55"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="101"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="30"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="30"/>
+      <c r="N13" s="15"/>
+    </row>
+    <row r="14" spans="1:14" ht="16" thickBot="1">
+      <c r="A14" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" s="70">
+        <v>41679</v>
+      </c>
+      <c r="C14" s="77">
+        <v>3</v>
+      </c>
+      <c r="D14" s="70">
+        <f t="shared" si="0"/>
+        <v>41700</v>
+      </c>
+      <c r="E14" s="102"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="46"/>
+      <c r="H14" s="110"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="30"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="30"/>
+      <c r="N14" s="15"/>
+    </row>
+    <row r="15" spans="1:14" ht="16" thickBot="1">
+      <c r="A15" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="70">
+        <v>41673</v>
+      </c>
+      <c r="C15" s="77">
+        <v>4</v>
+      </c>
+      <c r="D15" s="70">
+        <f t="shared" si="0"/>
+        <v>41701</v>
+      </c>
+      <c r="E15" s="111"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="47"/>
+      <c r="H15" s="112"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="30"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="30"/>
+      <c r="N15" s="15"/>
+    </row>
+    <row r="16" spans="1:14" ht="16" thickBot="1">
+      <c r="A16" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="70">
+        <v>41686</v>
+      </c>
+      <c r="C16" s="77">
+        <v>4</v>
+      </c>
+      <c r="D16" s="70">
+        <f t="shared" si="0"/>
+        <v>41714</v>
+      </c>
+      <c r="E16" s="102"/>
+      <c r="F16" s="61"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="112"/>
+      <c r="I16" s="47"/>
+      <c r="J16" s="56"/>
+      <c r="K16" s="30"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="30"/>
+      <c r="N16" s="15"/>
+    </row>
+    <row r="17" spans="1:14" ht="16" thickBot="1">
+      <c r="A17" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="70">
+        <v>41700</v>
+      </c>
+      <c r="C17" s="77">
+        <v>3</v>
+      </c>
+      <c r="D17" s="70">
+        <f t="shared" si="0"/>
+        <v>41721</v>
+      </c>
+      <c r="E17" s="104"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="63"/>
+      <c r="H17" s="101"/>
+      <c r="I17" s="90"/>
+      <c r="J17" s="31"/>
+      <c r="K17" s="54"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="30"/>
+      <c r="N17" s="15"/>
+    </row>
+    <row r="18" spans="1:14" ht="16" thickBot="1">
+      <c r="A18" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="71">
+        <v>41673</v>
+      </c>
+      <c r="C18" s="78">
+        <v>1</v>
+      </c>
+      <c r="D18" s="71">
+        <f t="shared" si="0"/>
+        <v>41680</v>
+      </c>
+      <c r="E18" s="113"/>
+      <c r="F18" s="60"/>
+      <c r="G18" s="62"/>
+      <c r="H18" s="101"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="30"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="30"/>
+      <c r="N18" s="15"/>
+    </row>
+    <row r="19" spans="1:14" ht="16" thickBot="1">
+      <c r="A19" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="71">
+        <v>41679</v>
+      </c>
+      <c r="C19" s="78">
+        <v>4</v>
+      </c>
+      <c r="D19" s="71">
+        <f t="shared" si="0"/>
+        <v>41707</v>
+      </c>
+      <c r="E19" s="114"/>
+      <c r="F19" s="82"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="115"/>
+      <c r="I19" s="91"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="30"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="30"/>
+      <c r="N19" s="15"/>
+    </row>
+    <row r="20" spans="1:14" ht="16" thickBot="1">
+      <c r="A20" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" s="71">
+        <v>41686</v>
+      </c>
+      <c r="C20" s="78">
+        <v>3</v>
+      </c>
+      <c r="D20" s="71">
+        <f t="shared" si="0"/>
+        <v>41707</v>
+      </c>
+      <c r="E20" s="104"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="43"/>
+      <c r="H20" s="116"/>
+      <c r="I20" s="91"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="30"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="30"/>
+      <c r="N20" s="15"/>
+    </row>
+    <row r="21" spans="1:14" ht="16" thickBot="1">
+      <c r="A21" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="71">
+        <v>41707</v>
+      </c>
+      <c r="C21" s="78">
+        <v>1</v>
+      </c>
+      <c r="D21" s="71">
+        <f t="shared" si="0"/>
+        <v>41714</v>
+      </c>
+      <c r="E21" s="104"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="30"/>
+      <c r="H21" s="101"/>
+      <c r="I21" s="16"/>
+      <c r="J21" s="59"/>
+      <c r="K21" s="15"/>
+      <c r="L21" s="14"/>
+      <c r="M21" s="30"/>
+      <c r="N21" s="15"/>
+    </row>
+    <row r="22" spans="1:14" ht="16" thickBot="1">
+      <c r="A22" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="66">
+        <v>41667</v>
+      </c>
+      <c r="C22" s="79">
+        <v>1</v>
+      </c>
+      <c r="D22" s="66">
+        <f t="shared" si="0"/>
+        <v>41674</v>
+      </c>
+      <c r="E22" s="104" t="s">
+        <v>62</v>
+      </c>
+      <c r="F22" s="14"/>
+      <c r="G22" s="30"/>
+      <c r="H22" s="101"/>
+      <c r="I22" s="92"/>
+      <c r="J22" s="16"/>
+      <c r="K22" s="30"/>
+      <c r="L22" s="14"/>
+      <c r="M22" s="30"/>
+      <c r="N22" s="15"/>
+    </row>
+    <row r="23" spans="1:14" ht="16" thickBot="1">
+      <c r="A23" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" s="66">
+        <v>41673</v>
+      </c>
+      <c r="C23" s="79">
+        <v>4</v>
+      </c>
+      <c r="D23" s="66">
+        <f t="shared" si="0"/>
+        <v>41701</v>
+      </c>
+      <c r="E23" s="117"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="35"/>
+      <c r="H23" s="118"/>
+      <c r="I23" s="92"/>
+      <c r="J23" s="16"/>
+      <c r="K23" s="30"/>
+      <c r="L23" s="14"/>
+      <c r="M23" s="30"/>
+      <c r="N23" s="15"/>
+    </row>
+    <row r="24" spans="1:14" ht="16" thickBot="1">
+      <c r="A24" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" s="66">
+        <v>41693</v>
+      </c>
+      <c r="C24" s="79">
+        <v>3</v>
+      </c>
+      <c r="D24" s="66">
+        <f t="shared" si="0"/>
+        <v>41714</v>
+      </c>
+      <c r="E24" s="104"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="30"/>
+      <c r="H24" s="118"/>
+      <c r="I24" s="93"/>
+      <c r="J24" s="23"/>
+      <c r="K24" s="34"/>
+      <c r="L24" s="14"/>
+      <c r="M24" s="30"/>
+      <c r="N24" s="15"/>
+    </row>
+    <row r="25" spans="1:14" ht="16" thickBot="1">
+      <c r="A25" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" s="72">
+        <v>41714</v>
+      </c>
+      <c r="C25" s="80">
+        <v>3</v>
+      </c>
+      <c r="D25" s="66">
+        <f t="shared" si="0"/>
+        <v>41735</v>
+      </c>
+      <c r="E25" s="119"/>
+      <c r="F25" s="120"/>
+      <c r="G25" s="121"/>
+      <c r="H25" s="122"/>
+      <c r="I25" s="94"/>
+      <c r="J25" s="18"/>
+      <c r="K25" s="35"/>
+      <c r="L25" s="23"/>
+      <c r="M25" s="35"/>
+      <c r="N25" s="19"/>
+    </row>
+    <row r="26" spans="1:14" ht="16" thickTop="1"/>
+    <row r="27" spans="1:14">
+      <c r="A27" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" s="13"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="85" t="s">
+        <v>41</v>
+      </c>
+      <c r="F27" s="85"/>
+    </row>
+    <row r="28" spans="1:14">
+      <c r="A28" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28" s="12"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="86" t="s">
+        <v>42</v>
+      </c>
+      <c r="F28" s="86"/>
+    </row>
+    <row r="29" spans="1:14">
+      <c r="A29" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="87" t="s">
         <v>38</v>
       </c>
-      <c r="K1" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="L1" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="M1" s="16" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="32" t="s">
-        <v>71</v>
-      </c>
-      <c r="B2" s="57"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="19"/>
-    </row>
-    <row r="3" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="59"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="41"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="41"/>
-      <c r="M3" s="19"/>
-    </row>
-    <row r="4" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="C4" s="18"/>
-      <c r="E4" s="59"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="41"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="41"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="41"/>
-      <c r="M4" s="19"/>
-    </row>
-    <row r="5" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="B5" s="19"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="49"/>
-      <c r="H5" s="41"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="41"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="41"/>
-      <c r="M5" s="19"/>
-    </row>
-    <row r="6" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="B6" s="19"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="41"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="60"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="41"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="41"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="41"/>
-      <c r="M6" s="19"/>
-    </row>
-    <row r="7" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="B7" s="19"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="59"/>
-      <c r="H7" s="59"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="41"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="41"/>
-      <c r="M7" s="19"/>
-    </row>
-    <row r="8" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="C8" s="18"/>
-      <c r="D8" s="41"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="59"/>
-      <c r="G8" s="59"/>
-      <c r="H8" s="41"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="41"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="41"/>
-      <c r="M8" s="19"/>
-    </row>
-    <row r="9" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="19"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="59"/>
-      <c r="G9" s="60"/>
-      <c r="H9" s="59"/>
-      <c r="J9" s="41"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="41"/>
-      <c r="M9" s="19"/>
-    </row>
-    <row r="10" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="19"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="41"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="41"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="41"/>
-      <c r="I10" s="60"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="41"/>
-      <c r="M10" s="19"/>
-    </row>
-    <row r="11" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="B11" s="19"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="41"/>
-      <c r="I11" s="61"/>
-      <c r="J11" s="61"/>
-      <c r="K11" s="18"/>
-      <c r="L11" s="41"/>
-      <c r="M11" s="19"/>
-    </row>
-    <row r="12" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="36"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="41"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="41"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="41"/>
-      <c r="K12" s="18"/>
-      <c r="L12" s="41"/>
-      <c r="M12" s="19"/>
-    </row>
-    <row r="13" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="19"/>
-      <c r="C13" s="35"/>
-      <c r="D13" s="42"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="41"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="41"/>
-      <c r="I13" s="18"/>
-      <c r="J13" s="41"/>
-      <c r="K13" s="18"/>
-      <c r="L13" s="41"/>
-      <c r="M13" s="19"/>
-    </row>
-    <row r="14" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="37"/>
-      <c r="C14" s="30"/>
-      <c r="D14" s="43"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="41"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="41"/>
-      <c r="I14" s="18"/>
-      <c r="J14" s="41"/>
-      <c r="K14" s="18"/>
-      <c r="L14" s="41"/>
-      <c r="M14" s="19"/>
-    </row>
-    <row r="15" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="51"/>
-      <c r="C15" s="52"/>
-      <c r="D15" s="43"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="43"/>
-      <c r="G15" s="30"/>
-      <c r="H15" s="41"/>
-      <c r="I15" s="18"/>
-      <c r="J15" s="41"/>
-      <c r="K15" s="18"/>
-      <c r="L15" s="41"/>
-      <c r="M15" s="19"/>
-    </row>
-    <row r="16" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="19"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="41"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="35"/>
-      <c r="G16" s="42"/>
-      <c r="H16" s="42"/>
-      <c r="I16" s="18"/>
-      <c r="J16" s="41"/>
-      <c r="K16" s="18"/>
-      <c r="L16" s="41"/>
-      <c r="M16" s="19"/>
-    </row>
-    <row r="17" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="26" t="s">
-        <v>62</v>
-      </c>
-      <c r="B17" s="38"/>
-      <c r="C17" s="29"/>
-      <c r="D17" s="44"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="41"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="41"/>
-      <c r="I17" s="18"/>
-      <c r="J17" s="41"/>
-      <c r="K17" s="18"/>
-      <c r="L17" s="41"/>
-      <c r="M17" s="19"/>
-    </row>
-    <row r="18" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="B18" s="19"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="45"/>
-      <c r="E18" s="29"/>
-      <c r="F18" s="29"/>
-      <c r="G18" s="29"/>
-      <c r="H18" s="44"/>
-      <c r="I18" s="18"/>
-      <c r="J18" s="41"/>
-      <c r="K18" s="18"/>
-      <c r="L18" s="41"/>
-      <c r="M18" s="19"/>
-    </row>
-    <row r="19" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="B19" s="19"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="41"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="41"/>
-      <c r="G19" s="29"/>
-      <c r="H19" s="44"/>
-      <c r="I19" s="18"/>
-      <c r="J19" s="41"/>
-      <c r="K19" s="18"/>
-      <c r="L19" s="41"/>
-      <c r="M19" s="19"/>
-    </row>
-    <row r="20" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="B20" s="19"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="41"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="41"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="45"/>
-      <c r="I20" s="29"/>
-      <c r="J20" s="41"/>
-      <c r="K20" s="18"/>
-      <c r="L20" s="41"/>
-      <c r="M20" s="19"/>
-    </row>
-    <row r="21" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="B21" s="39"/>
-      <c r="C21" s="28"/>
-      <c r="D21" s="41"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="41"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="45"/>
-      <c r="I21" s="20"/>
-      <c r="J21" s="41"/>
-      <c r="K21" s="18"/>
-      <c r="L21" s="41"/>
-      <c r="M21" s="19"/>
-    </row>
-    <row r="22" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="B22" s="19"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="46"/>
-      <c r="E22" s="28"/>
-      <c r="F22" s="46"/>
-      <c r="G22" s="28"/>
-      <c r="H22" s="45"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="41"/>
-      <c r="K22" s="18"/>
-      <c r="L22" s="41"/>
-      <c r="M22" s="19"/>
-    </row>
-    <row r="23" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="B23" s="19"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="41"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="41"/>
-      <c r="G23" s="28"/>
-      <c r="H23" s="46"/>
-      <c r="I23" s="28"/>
-      <c r="J23" s="45"/>
-      <c r="K23" s="18"/>
-      <c r="L23" s="41"/>
-      <c r="M23" s="19"/>
-    </row>
-    <row r="24" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="B24" s="23"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="47"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="47"/>
-      <c r="G24" s="21"/>
-      <c r="H24" s="50"/>
-      <c r="I24" s="22"/>
-      <c r="J24" s="46"/>
-      <c r="K24" s="28"/>
-      <c r="L24" s="46"/>
-      <c r="M24" s="23"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="B26" s="53" t="s">
-        <v>53</v>
-      </c>
-      <c r="C26" s="53"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="B27" s="54" t="s">
-        <v>54</v>
-      </c>
-      <c r="C27" s="54"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="11" t="s">
+      <c r="F29" s="87"/>
+    </row>
+    <row r="30" spans="1:14">
+      <c r="A30" s="84" t="s">
         <v>49</v>
       </c>
-      <c r="B28" s="55" t="s">
-        <v>50</v>
-      </c>
-      <c r="C28" s="55"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="56" t="s">
+      <c r="B30" s="84"/>
+      <c r="C30" s="84"/>
+      <c r="D30" s="84"/>
+      <c r="E30" s="84"/>
+      <c r="F30" s="84"/>
+    </row>
+    <row r="31" spans="1:14">
+      <c r="A31" s="83" t="s">
         <v>61</v>
       </c>
-      <c r="B29" s="56"/>
-      <c r="C29" s="56"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="58" t="s">
-        <v>72</v>
-      </c>
-      <c r="B30" s="58"/>
-      <c r="C30" s="58"/>
+      <c r="B31" s="83"/>
+      <c r="C31" s="83"/>
+      <c r="D31" s="83"/>
+      <c r="E31" s="83"/>
+      <c r="F31" s="83"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="A31:F31"/>
+    <mergeCell ref="A30:F30"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <colBreaks count="1" manualBreakCount="1">
-    <brk id="14" max="1048575" man="1"/>
+    <brk id="15" max="1048575" man="1"/>
   </colBreaks>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -2371,4 +3156,1368 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" customWidth="1"/>
+    <col min="3" max="3" width="9.5" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" customWidth="1"/>
+    <col min="5" max="14" width="9.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="30">
+      <c r="A1" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="73" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="73" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="73" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" s="88" t="s">
+        <v>73</v>
+      </c>
+      <c r="F1" s="88" t="s">
+        <v>74</v>
+      </c>
+      <c r="G1" s="88" t="s">
+        <v>75</v>
+      </c>
+      <c r="H1" s="88" t="s">
+        <v>76</v>
+      </c>
+      <c r="I1" s="88" t="s">
+        <v>77</v>
+      </c>
+      <c r="J1" s="88" t="s">
+        <v>78</v>
+      </c>
+      <c r="K1" s="88" t="s">
+        <v>79</v>
+      </c>
+      <c r="L1" s="88"/>
+      <c r="M1" s="88"/>
+      <c r="N1" s="88"/>
+    </row>
+    <row r="2" spans="1:14" ht="16" thickBot="1">
+      <c r="A2" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="67">
+        <v>41672</v>
+      </c>
+      <c r="C2" s="74">
+        <v>1</v>
+      </c>
+      <c r="D2" s="67">
+        <f>B2+C2*7</f>
+        <v>41679</v>
+      </c>
+      <c r="E2" s="65"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="15"/>
+    </row>
+    <row r="3" spans="1:14" ht="16" thickBot="1">
+      <c r="A3" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="68">
+        <v>41672</v>
+      </c>
+      <c r="C3" s="75">
+        <v>2</v>
+      </c>
+      <c r="D3" s="68">
+        <f t="shared" ref="D3:D24" si="0">B3+C3*7</f>
+        <v>41686</v>
+      </c>
+      <c r="E3" s="39"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="30"/>
+      <c r="N3" s="15"/>
+    </row>
+    <row r="4" spans="1:14" ht="16" thickBot="1">
+      <c r="A4" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="68">
+        <v>41679</v>
+      </c>
+      <c r="C4" s="75">
+        <v>2</v>
+      </c>
+      <c r="D4" s="68">
+        <f t="shared" si="0"/>
+        <v>41693</v>
+      </c>
+      <c r="E4" s="41"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="50"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="30"/>
+      <c r="N4" s="15"/>
+    </row>
+    <row r="5" spans="1:14" ht="16" thickBot="1">
+      <c r="A5" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" s="68">
+        <v>41672</v>
+      </c>
+      <c r="C5" s="75">
+        <v>2</v>
+      </c>
+      <c r="D5" s="68">
+        <f t="shared" si="0"/>
+        <v>41686</v>
+      </c>
+      <c r="E5" s="37"/>
+      <c r="F5" s="51"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="30"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="30"/>
+      <c r="N5" s="15"/>
+    </row>
+    <row r="6" spans="1:14" ht="16" thickBot="1">
+      <c r="A6" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" s="68">
+        <v>41686</v>
+      </c>
+      <c r="C6" s="75">
+        <v>1</v>
+      </c>
+      <c r="D6" s="68">
+        <f t="shared" si="0"/>
+        <v>41693</v>
+      </c>
+      <c r="E6" s="30"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="52"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="30"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="30"/>
+      <c r="N6" s="15"/>
+    </row>
+    <row r="7" spans="1:14" ht="16" thickBot="1">
+      <c r="A7" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" s="68">
+        <v>41693</v>
+      </c>
+      <c r="C7" s="75">
+        <v>2</v>
+      </c>
+      <c r="D7" s="68">
+        <f t="shared" si="0"/>
+        <v>41707</v>
+      </c>
+      <c r="E7" s="30"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="41"/>
+      <c r="H7" s="81"/>
+      <c r="I7" s="48"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="30"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="30"/>
+      <c r="N7" s="15"/>
+    </row>
+    <row r="8" spans="1:14" ht="16" thickBot="1">
+      <c r="A8" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" s="68">
+        <v>41686</v>
+      </c>
+      <c r="C8" s="75">
+        <v>2</v>
+      </c>
+      <c r="D8" s="68">
+        <f t="shared" si="0"/>
+        <v>41700</v>
+      </c>
+      <c r="E8" s="30"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="81"/>
+      <c r="H8" s="48"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="30"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="30"/>
+      <c r="N8" s="15"/>
+    </row>
+    <row r="9" spans="1:14" ht="16" thickBot="1">
+      <c r="A9" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="68">
+        <v>41686</v>
+      </c>
+      <c r="C9" s="75">
+        <v>3</v>
+      </c>
+      <c r="D9" s="68">
+        <f t="shared" si="0"/>
+        <v>41707</v>
+      </c>
+      <c r="E9" s="30"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="49"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="48"/>
+      <c r="K9" s="30"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="30"/>
+      <c r="N9" s="15"/>
+    </row>
+    <row r="10" spans="1:14" ht="16" thickBot="1">
+      <c r="A10" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="68">
+        <v>41707</v>
+      </c>
+      <c r="C10" s="75">
+        <v>1</v>
+      </c>
+      <c r="D10" s="68">
+        <f t="shared" si="0"/>
+        <v>41714</v>
+      </c>
+      <c r="E10" s="30"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="41"/>
+      <c r="J10" s="53"/>
+      <c r="L10" s="30"/>
+      <c r="M10" s="30"/>
+      <c r="N10" s="15"/>
+    </row>
+    <row r="11" spans="1:14" ht="16" thickBot="1">
+      <c r="A11" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" s="68">
+        <v>41707</v>
+      </c>
+      <c r="C11" s="75">
+        <v>2</v>
+      </c>
+      <c r="D11" s="68">
+        <f t="shared" si="0"/>
+        <v>41721</v>
+      </c>
+      <c r="E11" s="30"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="41"/>
+      <c r="J11" s="81"/>
+      <c r="K11" s="48"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="30"/>
+      <c r="N11" s="15"/>
+    </row>
+    <row r="12" spans="1:14" ht="16" hidden="1" thickBot="1">
+      <c r="A12" s="64" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="69"/>
+      <c r="C12" s="76" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" s="67" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E12" s="44"/>
+      <c r="F12" s="54"/>
+      <c r="G12" s="30"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="30"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="30"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="30"/>
+      <c r="N12" s="15"/>
+    </row>
+    <row r="13" spans="1:14" ht="16" thickBot="1">
+      <c r="A13" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" s="70">
+        <v>41673</v>
+      </c>
+      <c r="C13" s="77">
+        <v>2</v>
+      </c>
+      <c r="D13" s="70">
+        <f t="shared" si="0"/>
+        <v>41687</v>
+      </c>
+      <c r="E13" s="46"/>
+      <c r="F13" s="55"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="30"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="30"/>
+      <c r="N13" s="15"/>
+    </row>
+    <row r="14" spans="1:14" ht="16" thickBot="1">
+      <c r="A14" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" s="70">
+        <v>41679</v>
+      </c>
+      <c r="C14" s="77">
+        <v>3</v>
+      </c>
+      <c r="D14" s="70">
+        <f t="shared" si="0"/>
+        <v>41700</v>
+      </c>
+      <c r="E14" s="41"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="46"/>
+      <c r="H14" s="55"/>
+      <c r="I14" s="30"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="30"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="30"/>
+      <c r="N14" s="15"/>
+    </row>
+    <row r="15" spans="1:14" ht="16" thickBot="1">
+      <c r="A15" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="70">
+        <v>41673</v>
+      </c>
+      <c r="C15" s="77">
+        <v>4</v>
+      </c>
+      <c r="D15" s="70">
+        <f t="shared" si="0"/>
+        <v>41701</v>
+      </c>
+      <c r="E15" s="45"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="47"/>
+      <c r="H15" s="56"/>
+      <c r="I15" s="30"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="30"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="30"/>
+      <c r="N15" s="15"/>
+    </row>
+    <row r="16" spans="1:14" ht="16" thickBot="1">
+      <c r="A16" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="70">
+        <v>41686</v>
+      </c>
+      <c r="C16" s="77">
+        <v>4</v>
+      </c>
+      <c r="D16" s="70">
+        <f t="shared" si="0"/>
+        <v>41714</v>
+      </c>
+      <c r="E16" s="41"/>
+      <c r="F16" s="61"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="32"/>
+      <c r="J16" s="56"/>
+      <c r="K16" s="30"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="30"/>
+      <c r="N16" s="15"/>
+    </row>
+    <row r="17" spans="1:14" ht="16" thickBot="1">
+      <c r="A17" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="70">
+        <v>41700</v>
+      </c>
+      <c r="C17" s="77">
+        <v>3</v>
+      </c>
+      <c r="D17" s="70">
+        <f t="shared" si="0"/>
+        <v>41721</v>
+      </c>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="63"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="31"/>
+      <c r="K17" s="54"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="30"/>
+      <c r="N17" s="15"/>
+    </row>
+    <row r="18" spans="1:14" ht="16" thickBot="1">
+      <c r="A18" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="71">
+        <v>41673</v>
+      </c>
+      <c r="C18" s="78">
+        <v>1</v>
+      </c>
+      <c r="D18" s="71">
+        <f t="shared" si="0"/>
+        <v>41680</v>
+      </c>
+      <c r="E18" s="57"/>
+      <c r="F18" s="60"/>
+      <c r="G18" s="62"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="30"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="30"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="30"/>
+      <c r="N18" s="15"/>
+    </row>
+    <row r="19" spans="1:14" ht="16" thickBot="1">
+      <c r="A19" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="71">
+        <v>41679</v>
+      </c>
+      <c r="C19" s="78">
+        <v>4</v>
+      </c>
+      <c r="D19" s="71">
+        <f t="shared" si="0"/>
+        <v>41707</v>
+      </c>
+      <c r="E19" s="58"/>
+      <c r="F19" s="82"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="57"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="30"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="30"/>
+      <c r="N19" s="15"/>
+    </row>
+    <row r="20" spans="1:14" ht="16" thickBot="1">
+      <c r="A20" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" s="71">
+        <v>41686</v>
+      </c>
+      <c r="C20" s="78">
+        <v>3</v>
+      </c>
+      <c r="D20" s="71">
+        <f t="shared" si="0"/>
+        <v>41707</v>
+      </c>
+      <c r="E20" s="30"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="43"/>
+      <c r="H20" s="33"/>
+      <c r="I20" s="57"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="30"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="30"/>
+      <c r="N20" s="15"/>
+    </row>
+    <row r="21" spans="1:14" ht="16" thickBot="1">
+      <c r="A21" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="71">
+        <v>41707</v>
+      </c>
+      <c r="C21" s="78">
+        <v>1</v>
+      </c>
+      <c r="D21" s="71">
+        <f t="shared" si="0"/>
+        <v>41714</v>
+      </c>
+      <c r="E21" s="30"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="30"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="58"/>
+      <c r="J21" s="59"/>
+      <c r="K21" s="15"/>
+      <c r="L21" s="14"/>
+      <c r="M21" s="30"/>
+      <c r="N21" s="15"/>
+    </row>
+    <row r="22" spans="1:14" ht="16" thickBot="1">
+      <c r="A22" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" s="66">
+        <v>41673</v>
+      </c>
+      <c r="C22" s="79">
+        <v>4</v>
+      </c>
+      <c r="D22" s="66">
+        <f t="shared" si="0"/>
+        <v>41701</v>
+      </c>
+      <c r="E22" s="35"/>
+      <c r="F22" s="23"/>
+      <c r="G22" s="35"/>
+      <c r="H22" s="123"/>
+      <c r="I22" s="34"/>
+      <c r="J22" s="16"/>
+      <c r="K22" s="30"/>
+      <c r="L22" s="14"/>
+      <c r="M22" s="30"/>
+      <c r="N22" s="15"/>
+    </row>
+    <row r="23" spans="1:14" ht="16" thickBot="1">
+      <c r="A23" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B23" s="66">
+        <v>41693</v>
+      </c>
+      <c r="C23" s="79">
+        <v>3</v>
+      </c>
+      <c r="D23" s="66">
+        <f t="shared" si="0"/>
+        <v>41714</v>
+      </c>
+      <c r="E23" s="30"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="35"/>
+      <c r="I23" s="23"/>
+      <c r="K23" s="34"/>
+      <c r="L23" s="14"/>
+      <c r="M23" s="30"/>
+      <c r="N23" s="15"/>
+    </row>
+    <row r="24" spans="1:14" ht="16" thickBot="1">
+      <c r="A24" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24" s="72">
+        <v>41714</v>
+      </c>
+      <c r="C24" s="80">
+        <v>3</v>
+      </c>
+      <c r="D24" s="66">
+        <f t="shared" si="0"/>
+        <v>41735</v>
+      </c>
+      <c r="E24" s="36"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="36"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="38"/>
+      <c r="J24" s="35"/>
+      <c r="K24" s="23"/>
+      <c r="L24" s="35"/>
+      <c r="N24" s="19"/>
+    </row>
+    <row r="26" spans="1:14">
+      <c r="A26" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" s="13"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="85" t="s">
+        <v>41</v>
+      </c>
+      <c r="F26" s="85"/>
+    </row>
+    <row r="27" spans="1:14">
+      <c r="A27" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="86" t="s">
+        <v>42</v>
+      </c>
+      <c r="F27" s="86"/>
+    </row>
+    <row r="28" spans="1:14">
+      <c r="A28" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="87" t="s">
+        <v>38</v>
+      </c>
+      <c r="F28" s="87"/>
+    </row>
+    <row r="29" spans="1:14">
+      <c r="A29" s="84" t="s">
+        <v>49</v>
+      </c>
+      <c r="B29" s="84"/>
+      <c r="C29" s="84"/>
+      <c r="D29" s="84"/>
+      <c r="E29" s="84"/>
+      <c r="F29" s="84"/>
+    </row>
+    <row r="30" spans="1:14">
+      <c r="A30" s="83" t="s">
+        <v>61</v>
+      </c>
+      <c r="B30" s="83"/>
+      <c r="C30" s="83"/>
+      <c r="D30" s="83"/>
+      <c r="E30" s="83"/>
+      <c r="F30" s="83"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="A29:F29"/>
+    <mergeCell ref="A30:F30"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O30" sqref="O30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" customWidth="1"/>
+    <col min="3" max="3" width="9.5" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" customWidth="1"/>
+    <col min="5" max="14" width="9.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="30">
+      <c r="A1" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="73" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="73" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="73" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" s="88" t="s">
+        <v>73</v>
+      </c>
+      <c r="F1" s="88" t="s">
+        <v>74</v>
+      </c>
+      <c r="G1" s="88" t="s">
+        <v>75</v>
+      </c>
+      <c r="H1" s="88" t="s">
+        <v>76</v>
+      </c>
+      <c r="I1" s="88" t="s">
+        <v>77</v>
+      </c>
+      <c r="J1" s="88" t="s">
+        <v>78</v>
+      </c>
+      <c r="K1" s="88" t="s">
+        <v>79</v>
+      </c>
+      <c r="L1" s="88"/>
+      <c r="M1" s="88"/>
+      <c r="N1" s="88"/>
+    </row>
+    <row r="2" spans="1:14" ht="16" thickBot="1">
+      <c r="A2" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="67">
+        <v>41672</v>
+      </c>
+      <c r="C2" s="74">
+        <v>1</v>
+      </c>
+      <c r="D2" s="67">
+        <f>B2+C2*7</f>
+        <v>41679</v>
+      </c>
+      <c r="E2" s="65"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="15"/>
+    </row>
+    <row r="3" spans="1:14" ht="16" thickBot="1">
+      <c r="A3" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="68">
+        <v>41672</v>
+      </c>
+      <c r="C3" s="75">
+        <v>2</v>
+      </c>
+      <c r="D3" s="68">
+        <f t="shared" ref="D3:D23" si="0">B3+C3*7</f>
+        <v>41686</v>
+      </c>
+      <c r="E3" s="39"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="30"/>
+      <c r="N3" s="15"/>
+    </row>
+    <row r="4" spans="1:14" ht="16" thickBot="1">
+      <c r="A4" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="68">
+        <v>41679</v>
+      </c>
+      <c r="C4" s="75">
+        <v>2</v>
+      </c>
+      <c r="D4" s="68">
+        <f t="shared" si="0"/>
+        <v>41693</v>
+      </c>
+      <c r="E4" s="41"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="50"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="30"/>
+      <c r="N4" s="15"/>
+    </row>
+    <row r="5" spans="1:14" ht="16" thickBot="1">
+      <c r="A5" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" s="68">
+        <v>41672</v>
+      </c>
+      <c r="C5" s="75">
+        <v>2</v>
+      </c>
+      <c r="D5" s="68">
+        <f t="shared" si="0"/>
+        <v>41686</v>
+      </c>
+      <c r="E5" s="37"/>
+      <c r="F5" s="51"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="30"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="30"/>
+      <c r="N5" s="15"/>
+    </row>
+    <row r="6" spans="1:14" ht="16" thickBot="1">
+      <c r="A6" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" s="68">
+        <v>41686</v>
+      </c>
+      <c r="C6" s="75">
+        <v>1</v>
+      </c>
+      <c r="D6" s="68">
+        <f t="shared" si="0"/>
+        <v>41693</v>
+      </c>
+      <c r="E6" s="30"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="52"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="30"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="30"/>
+      <c r="N6" s="15"/>
+    </row>
+    <row r="7" spans="1:14" ht="16" thickBot="1">
+      <c r="A7" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" s="68">
+        <v>41693</v>
+      </c>
+      <c r="C7" s="75">
+        <v>2</v>
+      </c>
+      <c r="D7" s="68">
+        <f t="shared" si="0"/>
+        <v>41707</v>
+      </c>
+      <c r="E7" s="30"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="41"/>
+      <c r="H7" s="81"/>
+      <c r="I7" s="48"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="30"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="30"/>
+      <c r="N7" s="15"/>
+    </row>
+    <row r="8" spans="1:14" ht="16" thickBot="1">
+      <c r="A8" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" s="68">
+        <v>41686</v>
+      </c>
+      <c r="C8" s="75">
+        <v>2</v>
+      </c>
+      <c r="D8" s="68">
+        <f t="shared" si="0"/>
+        <v>41700</v>
+      </c>
+      <c r="E8" s="30"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="81"/>
+      <c r="H8" s="48"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="30"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="30"/>
+      <c r="N8" s="15"/>
+    </row>
+    <row r="9" spans="1:14" ht="16" thickBot="1">
+      <c r="A9" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="68">
+        <v>41686</v>
+      </c>
+      <c r="C9" s="75">
+        <v>3</v>
+      </c>
+      <c r="D9" s="68">
+        <f t="shared" si="0"/>
+        <v>41707</v>
+      </c>
+      <c r="E9" s="30"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="49"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="48"/>
+      <c r="K9" s="30"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="30"/>
+      <c r="N9" s="15"/>
+    </row>
+    <row r="10" spans="1:14" ht="16" thickBot="1">
+      <c r="A10" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="68">
+        <v>41707</v>
+      </c>
+      <c r="C10" s="75">
+        <v>1</v>
+      </c>
+      <c r="D10" s="68">
+        <f t="shared" si="0"/>
+        <v>41714</v>
+      </c>
+      <c r="E10" s="30"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="41"/>
+      <c r="J10" s="53"/>
+      <c r="L10" s="30"/>
+      <c r="M10" s="30"/>
+      <c r="N10" s="15"/>
+    </row>
+    <row r="11" spans="1:14" ht="16" thickBot="1">
+      <c r="A11" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" s="68">
+        <v>41707</v>
+      </c>
+      <c r="C11" s="75">
+        <v>2</v>
+      </c>
+      <c r="D11" s="68">
+        <f t="shared" si="0"/>
+        <v>41721</v>
+      </c>
+      <c r="E11" s="30"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="41"/>
+      <c r="J11" s="81"/>
+      <c r="K11" s="48"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="30"/>
+      <c r="N11" s="15"/>
+    </row>
+    <row r="12" spans="1:14" ht="16" hidden="1" thickBot="1">
+      <c r="A12" s="64" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="69"/>
+      <c r="C12" s="76" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" s="67" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E12" s="44"/>
+      <c r="F12" s="54"/>
+      <c r="G12" s="30"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="30"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="30"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="30"/>
+      <c r="N12" s="15"/>
+    </row>
+    <row r="13" spans="1:14" ht="16" thickBot="1">
+      <c r="A13" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" s="70">
+        <v>41673</v>
+      </c>
+      <c r="C13" s="77">
+        <v>2</v>
+      </c>
+      <c r="D13" s="70">
+        <f t="shared" si="0"/>
+        <v>41687</v>
+      </c>
+      <c r="E13" s="46"/>
+      <c r="F13" s="55"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="30"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="30"/>
+      <c r="N13" s="15"/>
+    </row>
+    <row r="14" spans="1:14" ht="16" thickBot="1">
+      <c r="A14" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" s="70">
+        <v>41679</v>
+      </c>
+      <c r="C14" s="77">
+        <v>3</v>
+      </c>
+      <c r="D14" s="70">
+        <f t="shared" si="0"/>
+        <v>41700</v>
+      </c>
+      <c r="E14" s="41"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="46"/>
+      <c r="H14" s="55"/>
+      <c r="I14" s="30"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="30"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="30"/>
+      <c r="N14" s="15"/>
+    </row>
+    <row r="15" spans="1:14" ht="16" thickBot="1">
+      <c r="A15" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="70">
+        <v>41673</v>
+      </c>
+      <c r="C15" s="77">
+        <v>4</v>
+      </c>
+      <c r="D15" s="70">
+        <f t="shared" si="0"/>
+        <v>41701</v>
+      </c>
+      <c r="E15" s="45"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="47"/>
+      <c r="H15" s="56"/>
+      <c r="I15" s="30"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="30"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="30"/>
+      <c r="N15" s="15"/>
+    </row>
+    <row r="16" spans="1:14" ht="16" thickBot="1">
+      <c r="A16" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="70">
+        <v>41686</v>
+      </c>
+      <c r="C16" s="77">
+        <v>4</v>
+      </c>
+      <c r="D16" s="70">
+        <f t="shared" si="0"/>
+        <v>41714</v>
+      </c>
+      <c r="E16" s="41"/>
+      <c r="F16" s="61"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="32"/>
+      <c r="J16" s="56"/>
+      <c r="K16" s="30"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="30"/>
+      <c r="N16" s="15"/>
+    </row>
+    <row r="17" spans="1:14" ht="16" thickBot="1">
+      <c r="A17" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="70">
+        <v>41700</v>
+      </c>
+      <c r="C17" s="77">
+        <v>3</v>
+      </c>
+      <c r="D17" s="70">
+        <f t="shared" si="0"/>
+        <v>41721</v>
+      </c>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="63"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="31"/>
+      <c r="K17" s="54"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="30"/>
+      <c r="N17" s="15"/>
+    </row>
+    <row r="18" spans="1:14" ht="16" thickBot="1">
+      <c r="A18" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" s="71">
+        <v>41679</v>
+      </c>
+      <c r="C18" s="78">
+        <v>4</v>
+      </c>
+      <c r="D18" s="71">
+        <f t="shared" si="0"/>
+        <v>41707</v>
+      </c>
+      <c r="E18" s="124"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="57"/>
+      <c r="K18" s="30"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="30"/>
+      <c r="N18" s="15"/>
+    </row>
+    <row r="19" spans="1:14" ht="16" thickBot="1">
+      <c r="A19" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" s="71">
+        <v>41686</v>
+      </c>
+      <c r="C19" s="78">
+        <v>3</v>
+      </c>
+      <c r="D19" s="71">
+        <f t="shared" si="0"/>
+        <v>41707</v>
+      </c>
+      <c r="E19" s="59"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="125"/>
+      <c r="H19" s="82"/>
+      <c r="I19" s="57"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="30"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="30"/>
+      <c r="N19" s="15"/>
+    </row>
+    <row r="20" spans="1:14" ht="16" thickBot="1">
+      <c r="A20" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="71">
+        <v>41707</v>
+      </c>
+      <c r="C20" s="78">
+        <v>1</v>
+      </c>
+      <c r="D20" s="71">
+        <f t="shared" si="0"/>
+        <v>41714</v>
+      </c>
+      <c r="E20" s="124"/>
+      <c r="F20" s="126"/>
+      <c r="G20" s="127"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="58"/>
+      <c r="J20" s="30"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="30"/>
+      <c r="N20" s="15"/>
+    </row>
+    <row r="21" spans="1:14" ht="16" thickBot="1">
+      <c r="A21" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" s="66">
+        <v>41673</v>
+      </c>
+      <c r="C21" s="79">
+        <v>4</v>
+      </c>
+      <c r="D21" s="66">
+        <f t="shared" si="0"/>
+        <v>41701</v>
+      </c>
+      <c r="E21" s="128"/>
+      <c r="F21" s="35"/>
+      <c r="G21" s="129"/>
+      <c r="H21" s="60"/>
+      <c r="I21" s="34"/>
+      <c r="J21" s="16"/>
+      <c r="K21" s="30"/>
+      <c r="L21" s="14"/>
+      <c r="M21" s="30"/>
+      <c r="N21" s="15"/>
+    </row>
+    <row r="22" spans="1:14" ht="16" thickBot="1">
+      <c r="A22" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" s="66">
+        <v>41693</v>
+      </c>
+      <c r="C22" s="79">
+        <v>3</v>
+      </c>
+      <c r="D22" s="66">
+        <f t="shared" si="0"/>
+        <v>41714</v>
+      </c>
+      <c r="E22" s="30"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="130"/>
+      <c r="H22" s="35"/>
+      <c r="I22" s="131"/>
+      <c r="K22" s="34"/>
+      <c r="L22" s="14"/>
+      <c r="M22" s="30"/>
+      <c r="N22" s="15"/>
+    </row>
+    <row r="23" spans="1:14" ht="16" thickBot="1">
+      <c r="A23" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" s="72">
+        <v>41714</v>
+      </c>
+      <c r="C23" s="80">
+        <v>3</v>
+      </c>
+      <c r="D23" s="66">
+        <f t="shared" si="0"/>
+        <v>41735</v>
+      </c>
+      <c r="E23" s="36"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="36"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="38"/>
+      <c r="J23" s="35"/>
+      <c r="K23" s="23"/>
+      <c r="L23" s="35"/>
+      <c r="M23" s="36"/>
+      <c r="N23" s="19"/>
+    </row>
+    <row r="25" spans="1:14">
+      <c r="A25" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="85" t="s">
+        <v>41</v>
+      </c>
+      <c r="F25" s="85"/>
+    </row>
+    <row r="26" spans="1:14">
+      <c r="A26" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="86" t="s">
+        <v>42</v>
+      </c>
+      <c r="F26" s="86"/>
+    </row>
+    <row r="27" spans="1:14">
+      <c r="A27" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="87" t="s">
+        <v>38</v>
+      </c>
+      <c r="F27" s="87"/>
+    </row>
+    <row r="28" spans="1:14">
+      <c r="A28" s="84" t="s">
+        <v>49</v>
+      </c>
+      <c r="B28" s="84"/>
+      <c r="C28" s="84"/>
+      <c r="D28" s="84"/>
+      <c r="E28" s="84"/>
+      <c r="F28" s="84"/>
+    </row>
+    <row r="29" spans="1:14">
+      <c r="A29" s="83" t="s">
+        <v>61</v>
+      </c>
+      <c r="B29" s="83"/>
+      <c r="C29" s="83"/>
+      <c r="D29" s="83"/>
+      <c r="E29" s="83"/>
+      <c r="F29" s="83"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="A28:F28"/>
+    <mergeCell ref="A29:F29"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
hardware groups updated schedule
</commit_message>
<xml_diff>
--- a/Admin stuff/ganttChart copy.xlsx
+++ b/Admin stuff/ganttChart copy.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-33540" yWindow="-4660" windowWidth="24720" windowHeight="15460" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="1760" yWindow="1320" windowWidth="36140" windowHeight="20300" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="90">
   <si>
     <t>Task</t>
   </si>
@@ -275,6 +275,37 @@
   <si>
     <t>Week 13
 4/13</t>
+  </si>
+  <si>
+    <t>https://github.com/gconan/GroBot_DesignFiles.git</t>
+  </si>
+  <si>
+    <t>Week 14
+4/20</t>
+  </si>
+  <si>
+    <t>Order Lights, Water Pumps, Sockets, Fuses</t>
+  </si>
+  <si>
+    <t>Akinwande and Fred about PCB and soldering</t>
+  </si>
+  <si>
+    <t>Test Water and Air w and w/o uC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Order components for Buck </t>
+  </si>
+  <si>
+    <t>PCB Design</t>
+  </si>
+  <si>
+    <t>PCB Order</t>
+  </si>
+  <si>
+    <t>Testing and Integration</t>
+  </si>
+  <si>
+    <t>DC Auxilary Drivers</t>
   </si>
 </sst>
 </file>
@@ -2423,9 +2454,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView zoomScale="104" zoomScaleNormal="104" zoomScalePageLayoutView="104" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I27" sqref="I27"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2:H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3162,7 +3193,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
@@ -3854,10 +3885,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N29"/>
+  <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O30" sqref="O30"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3871,7 +3902,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="30">
       <c r="A1" s="40" t="s">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="B1" s="73" t="s">
         <v>65</v>
@@ -3903,13 +3934,15 @@
       <c r="K1" s="88" t="s">
         <v>79</v>
       </c>
-      <c r="L1" s="88"/>
+      <c r="L1" s="88" t="s">
+        <v>81</v>
+      </c>
       <c r="M1" s="88"/>
       <c r="N1" s="88"/>
     </row>
     <row r="2" spans="1:14" ht="16" thickBot="1">
       <c r="A2" s="26" t="s">
-        <v>59</v>
+        <v>82</v>
       </c>
       <c r="B2" s="67">
         <v>41672</v>
@@ -3934,21 +3967,21 @@
     </row>
     <row r="3" spans="1:14" ht="16" thickBot="1">
       <c r="A3" s="26" t="s">
-        <v>54</v>
+        <v>83</v>
       </c>
       <c r="B3" s="68">
         <v>41672</v>
       </c>
       <c r="C3" s="75">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3" s="68">
-        <f t="shared" ref="D3:D23" si="0">B3+C3*7</f>
-        <v>41686</v>
-      </c>
-      <c r="E3" s="39"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="15"/>
+        <f t="shared" ref="D3:D8" si="0">B3+C3*7</f>
+        <v>41679</v>
+      </c>
+      <c r="E3" s="65"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
       <c r="H3" s="14"/>
       <c r="I3" s="30"/>
       <c r="J3" s="14"/>
@@ -3959,7 +3992,7 @@
     </row>
     <row r="4" spans="1:14" ht="16" thickBot="1">
       <c r="A4" s="26" t="s">
-        <v>53</v>
+        <v>84</v>
       </c>
       <c r="B4" s="68">
         <v>41679</v>
@@ -3971,9 +4004,8 @@
         <f t="shared" si="0"/>
         <v>41693</v>
       </c>
-      <c r="E4" s="41"/>
-      <c r="F4" s="49"/>
-      <c r="G4" s="50"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="50"/>
       <c r="H4" s="14"/>
       <c r="I4" s="30"/>
       <c r="J4" s="14"/>
@@ -3984,7 +4016,7 @@
     </row>
     <row r="5" spans="1:14" ht="16" thickBot="1">
       <c r="A5" s="26" t="s">
-        <v>55</v>
+        <v>85</v>
       </c>
       <c r="B5" s="68">
         <v>41672</v>
@@ -3996,8 +4028,8 @@
         <f t="shared" si="0"/>
         <v>41686</v>
       </c>
-      <c r="E5" s="37"/>
-      <c r="F5" s="51"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="50"/>
       <c r="I5" s="30"/>
       <c r="J5" s="14"/>
       <c r="K5" s="30"/>
@@ -4007,22 +4039,14 @@
     </row>
     <row r="6" spans="1:14" ht="16" thickBot="1">
       <c r="A6" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="B6" s="68">
-        <v>41686</v>
-      </c>
-      <c r="C6" s="75">
-        <v>1</v>
-      </c>
-      <c r="D6" s="68">
-        <f t="shared" si="0"/>
-        <v>41693</v>
-      </c>
-      <c r="E6" s="30"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="52"/>
-      <c r="H6" s="14"/>
+        <v>86</v>
+      </c>
+      <c r="B6" s="68"/>
+      <c r="C6" s="75"/>
+      <c r="D6" s="68"/>
+      <c r="E6" s="49"/>
+      <c r="F6" s="49"/>
+      <c r="G6" s="49"/>
       <c r="I6" s="30"/>
       <c r="J6" s="14"/>
       <c r="K6" s="30"/>
@@ -4032,23 +4056,22 @@
     </row>
     <row r="7" spans="1:14" ht="16" thickBot="1">
       <c r="A7" s="26" t="s">
-        <v>56</v>
+        <v>87</v>
       </c>
       <c r="B7" s="68">
+        <v>41686</v>
+      </c>
+      <c r="C7" s="75">
+        <v>1</v>
+      </c>
+      <c r="D7" s="68">
+        <f t="shared" si="0"/>
         <v>41693</v>
-      </c>
-      <c r="C7" s="75">
-        <v>2</v>
-      </c>
-      <c r="D7" s="68">
-        <f t="shared" si="0"/>
-        <v>41707</v>
       </c>
       <c r="E7" s="30"/>
       <c r="F7" s="14"/>
-      <c r="G7" s="41"/>
-      <c r="H7" s="81"/>
-      <c r="I7" s="48"/>
+      <c r="G7" s="52"/>
+      <c r="I7" s="30"/>
       <c r="J7" s="14"/>
       <c r="K7" s="30"/>
       <c r="L7" s="14"/>
@@ -4057,169 +4080,172 @@
     </row>
     <row r="8" spans="1:14" ht="16" thickBot="1">
       <c r="A8" s="26" t="s">
-        <v>58</v>
+        <v>88</v>
       </c>
       <c r="B8" s="68">
-        <v>41686</v>
+        <v>41693</v>
       </c>
       <c r="C8" s="75">
         <v>2</v>
       </c>
       <c r="D8" s="68">
         <f t="shared" si="0"/>
-        <v>41700</v>
+        <v>41707</v>
       </c>
       <c r="E8" s="30"/>
       <c r="F8" s="14"/>
-      <c r="G8" s="81"/>
-      <c r="H8" s="48"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="30"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="81"/>
+      <c r="I8" s="48"/>
+      <c r="J8" s="48"/>
+      <c r="K8" s="48"/>
       <c r="L8" s="14"/>
       <c r="M8" s="30"/>
       <c r="N8" s="15"/>
     </row>
     <row r="9" spans="1:14" ht="16" thickBot="1">
-      <c r="A9" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="68">
-        <v>41686</v>
-      </c>
-      <c r="C9" s="75">
+      <c r="A9" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="B9" s="70">
+        <v>41679</v>
+      </c>
+      <c r="C9" s="77">
         <v>3</v>
       </c>
-      <c r="D9" s="68">
-        <f t="shared" si="0"/>
-        <v>41707</v>
-      </c>
-      <c r="E9" s="30"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="49"/>
-      <c r="H9" s="39"/>
-      <c r="I9" s="48"/>
+      <c r="D9" s="70">
+        <f t="shared" ref="D9:D18" si="1">B9+C9*7</f>
+        <v>41700</v>
+      </c>
+      <c r="E9" s="41"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="46"/>
+      <c r="H9" s="55"/>
+      <c r="I9" s="30"/>
+      <c r="J9" s="14"/>
       <c r="K9" s="30"/>
       <c r="L9" s="14"/>
       <c r="M9" s="30"/>
       <c r="N9" s="15"/>
     </row>
     <row r="10" spans="1:14" ht="16" thickBot="1">
-      <c r="A10" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="68">
-        <v>41707</v>
-      </c>
-      <c r="C10" s="75">
-        <v>1</v>
-      </c>
-      <c r="D10" s="68">
-        <f t="shared" si="0"/>
-        <v>41714</v>
-      </c>
-      <c r="E10" s="30"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="41"/>
-      <c r="J10" s="53"/>
-      <c r="L10" s="30"/>
+      <c r="A10" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="70">
+        <v>41673</v>
+      </c>
+      <c r="C10" s="77">
+        <v>4</v>
+      </c>
+      <c r="D10" s="70">
+        <f t="shared" si="1"/>
+        <v>41701</v>
+      </c>
+      <c r="E10" s="45"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="47"/>
+      <c r="H10" s="56"/>
+      <c r="I10" s="30"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="30"/>
+      <c r="L10" s="14"/>
       <c r="M10" s="30"/>
       <c r="N10" s="15"/>
     </row>
     <row r="11" spans="1:14" ht="16" thickBot="1">
-      <c r="A11" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="B11" s="68">
-        <v>41707</v>
-      </c>
-      <c r="C11" s="75">
-        <v>2</v>
-      </c>
-      <c r="D11" s="68">
-        <f t="shared" si="0"/>
-        <v>41721</v>
-      </c>
-      <c r="E11" s="30"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="30"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="41"/>
-      <c r="J11" s="81"/>
-      <c r="K11" s="48"/>
+      <c r="A11" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="70">
+        <v>41686</v>
+      </c>
+      <c r="C11" s="77">
+        <v>4</v>
+      </c>
+      <c r="D11" s="70">
+        <f t="shared" si="1"/>
+        <v>41714</v>
+      </c>
+      <c r="E11" s="41"/>
+      <c r="F11" s="61"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="56"/>
+      <c r="K11" s="30"/>
       <c r="L11" s="14"/>
       <c r="M11" s="30"/>
       <c r="N11" s="15"/>
     </row>
-    <row r="12" spans="1:14" ht="16" hidden="1" thickBot="1">
-      <c r="A12" s="64" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="69"/>
-      <c r="C12" s="76" t="s">
-        <v>67</v>
-      </c>
-      <c r="D12" s="67" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E12" s="44"/>
-      <c r="F12" s="54"/>
-      <c r="G12" s="30"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="30"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="30"/>
+    <row r="12" spans="1:14" ht="16" thickBot="1">
+      <c r="A12" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="70">
+        <v>41700</v>
+      </c>
+      <c r="C12" s="77">
+        <v>3</v>
+      </c>
+      <c r="D12" s="70">
+        <f t="shared" si="1"/>
+        <v>41721</v>
+      </c>
+      <c r="E12" s="30"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="63"/>
+      <c r="I12" s="42"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="54"/>
       <c r="L12" s="14"/>
       <c r="M12" s="30"/>
       <c r="N12" s="15"/>
     </row>
     <row r="13" spans="1:14" ht="16" thickBot="1">
-      <c r="A13" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="B13" s="70">
-        <v>41673</v>
-      </c>
-      <c r="C13" s="77">
-        <v>2</v>
-      </c>
-      <c r="D13" s="70">
-        <f t="shared" si="0"/>
-        <v>41687</v>
-      </c>
-      <c r="E13" s="46"/>
-      <c r="F13" s="55"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="30"/>
-      <c r="J13" s="14"/>
+      <c r="A13" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" s="71">
+        <v>41679</v>
+      </c>
+      <c r="C13" s="78">
+        <v>4</v>
+      </c>
+      <c r="D13" s="71">
+        <f t="shared" si="1"/>
+        <v>41707</v>
+      </c>
+      <c r="E13" s="124"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="33"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="33"/>
+      <c r="J13" s="57"/>
       <c r="K13" s="30"/>
       <c r="L13" s="14"/>
       <c r="M13" s="30"/>
       <c r="N13" s="15"/>
     </row>
     <row r="14" spans="1:14" ht="16" thickBot="1">
-      <c r="A14" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="B14" s="70">
-        <v>41679</v>
-      </c>
-      <c r="C14" s="77">
+      <c r="A14" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" s="71">
+        <v>41686</v>
+      </c>
+      <c r="C14" s="78">
         <v>3</v>
       </c>
-      <c r="D14" s="70">
-        <f t="shared" si="0"/>
-        <v>41700</v>
-      </c>
-      <c r="E14" s="41"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="46"/>
-      <c r="H14" s="55"/>
-      <c r="I14" s="30"/>
+      <c r="D14" s="71">
+        <f t="shared" si="1"/>
+        <v>41707</v>
+      </c>
+      <c r="E14" s="59"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="125"/>
+      <c r="H14" s="82"/>
+      <c r="I14" s="57"/>
       <c r="J14" s="14"/>
       <c r="K14" s="30"/>
       <c r="L14" s="14"/>
@@ -4227,291 +4253,167 @@
       <c r="N14" s="15"/>
     </row>
     <row r="15" spans="1:14" ht="16" thickBot="1">
-      <c r="A15" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="70">
-        <v>41673</v>
-      </c>
-      <c r="C15" s="77">
-        <v>4</v>
-      </c>
-      <c r="D15" s="70">
-        <f t="shared" si="0"/>
-        <v>41701</v>
-      </c>
-      <c r="E15" s="45"/>
-      <c r="F15" s="32"/>
-      <c r="G15" s="47"/>
-      <c r="H15" s="56"/>
-      <c r="I15" s="30"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="30"/>
+      <c r="A15" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="71">
+        <v>41707</v>
+      </c>
+      <c r="C15" s="78">
+        <v>1</v>
+      </c>
+      <c r="D15" s="71">
+        <f t="shared" si="1"/>
+        <v>41714</v>
+      </c>
+      <c r="E15" s="124"/>
+      <c r="F15" s="126"/>
+      <c r="G15" s="127"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="58"/>
+      <c r="J15" s="30"/>
+      <c r="K15" s="15"/>
       <c r="L15" s="14"/>
       <c r="M15" s="30"/>
       <c r="N15" s="15"/>
     </row>
     <row r="16" spans="1:14" ht="16" thickBot="1">
-      <c r="A16" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="70">
-        <v>41686</v>
-      </c>
-      <c r="C16" s="77">
+      <c r="A16" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="66">
+        <v>41673</v>
+      </c>
+      <c r="C16" s="79">
         <v>4</v>
       </c>
-      <c r="D16" s="70">
-        <f t="shared" si="0"/>
-        <v>41714</v>
-      </c>
-      <c r="E16" s="41"/>
-      <c r="F16" s="61"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="25"/>
-      <c r="I16" s="32"/>
-      <c r="J16" s="56"/>
+      <c r="D16" s="66">
+        <f t="shared" si="1"/>
+        <v>41701</v>
+      </c>
+      <c r="E16" s="128"/>
+      <c r="F16" s="35"/>
+      <c r="G16" s="129"/>
+      <c r="H16" s="60"/>
+      <c r="I16" s="34"/>
+      <c r="J16" s="16"/>
       <c r="K16" s="30"/>
       <c r="L16" s="14"/>
       <c r="M16" s="30"/>
       <c r="N16" s="15"/>
     </row>
     <row r="17" spans="1:14" ht="16" thickBot="1">
-      <c r="A17" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" s="70">
-        <v>41700</v>
-      </c>
-      <c r="C17" s="77">
+      <c r="A17" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="66">
+        <v>41693</v>
+      </c>
+      <c r="C17" s="79">
         <v>3</v>
       </c>
-      <c r="D17" s="70">
-        <f t="shared" si="0"/>
-        <v>41721</v>
+      <c r="D17" s="66">
+        <f t="shared" si="1"/>
+        <v>41714</v>
       </c>
       <c r="E17" s="30"/>
-      <c r="F17" s="30"/>
-      <c r="G17" s="63"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="31"/>
-      <c r="K17" s="54"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="130"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="131"/>
+      <c r="K17" s="34"/>
       <c r="L17" s="14"/>
       <c r="M17" s="30"/>
       <c r="N17" s="15"/>
     </row>
     <row r="18" spans="1:14" ht="16" thickBot="1">
-      <c r="A18" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="B18" s="71">
-        <v>41679</v>
-      </c>
-      <c r="C18" s="78">
-        <v>4</v>
-      </c>
-      <c r="D18" s="71">
-        <f t="shared" si="0"/>
-        <v>41707</v>
-      </c>
-      <c r="E18" s="124"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="33"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
-      <c r="J18" s="57"/>
-      <c r="K18" s="30"/>
-      <c r="L18" s="14"/>
-      <c r="M18" s="30"/>
-      <c r="N18" s="15"/>
-    </row>
-    <row r="19" spans="1:14" ht="16" thickBot="1">
-      <c r="A19" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="B19" s="71">
-        <v>41686</v>
-      </c>
-      <c r="C19" s="78">
+      <c r="A18" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="72">
+        <v>41714</v>
+      </c>
+      <c r="C18" s="80">
         <v>3</v>
       </c>
-      <c r="D19" s="71">
-        <f t="shared" si="0"/>
-        <v>41707</v>
-      </c>
-      <c r="E19" s="59"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="125"/>
-      <c r="H19" s="82"/>
-      <c r="I19" s="57"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="30"/>
-      <c r="L19" s="14"/>
-      <c r="M19" s="30"/>
-      <c r="N19" s="15"/>
-    </row>
-    <row r="20" spans="1:14" ht="16" thickBot="1">
-      <c r="A20" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="B20" s="71">
-        <v>41707</v>
-      </c>
-      <c r="C20" s="78">
-        <v>1</v>
-      </c>
-      <c r="D20" s="71">
-        <f t="shared" si="0"/>
-        <v>41714</v>
-      </c>
-      <c r="E20" s="124"/>
-      <c r="F20" s="126"/>
-      <c r="G20" s="127"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="58"/>
-      <c r="J20" s="30"/>
-      <c r="K20" s="15"/>
-      <c r="L20" s="14"/>
-      <c r="M20" s="30"/>
-      <c r="N20" s="15"/>
-    </row>
-    <row r="21" spans="1:14" ht="16" thickBot="1">
-      <c r="A21" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="B21" s="66">
-        <v>41673</v>
-      </c>
-      <c r="C21" s="79">
-        <v>4</v>
-      </c>
-      <c r="D21" s="66">
-        <f t="shared" si="0"/>
-        <v>41701</v>
-      </c>
-      <c r="E21" s="128"/>
-      <c r="F21" s="35"/>
-      <c r="G21" s="129"/>
-      <c r="H21" s="60"/>
-      <c r="I21" s="34"/>
-      <c r="J21" s="16"/>
-      <c r="K21" s="30"/>
-      <c r="L21" s="14"/>
-      <c r="M21" s="30"/>
-      <c r="N21" s="15"/>
-    </row>
-    <row r="22" spans="1:14" ht="16" thickBot="1">
-      <c r="A22" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="B22" s="66">
-        <v>41693</v>
-      </c>
-      <c r="C22" s="79">
-        <v>3</v>
-      </c>
-      <c r="D22" s="66">
-        <f t="shared" si="0"/>
-        <v>41714</v>
-      </c>
-      <c r="E22" s="30"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="130"/>
-      <c r="H22" s="35"/>
-      <c r="I22" s="131"/>
-      <c r="K22" s="34"/>
-      <c r="L22" s="14"/>
-      <c r="M22" s="30"/>
-      <c r="N22" s="15"/>
-    </row>
-    <row r="23" spans="1:14" ht="16" thickBot="1">
-      <c r="A23" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="B23" s="72">
-        <v>41714</v>
-      </c>
-      <c r="C23" s="80">
-        <v>3</v>
-      </c>
-      <c r="D23" s="66">
-        <f t="shared" si="0"/>
+      <c r="D18" s="66">
+        <f t="shared" si="1"/>
         <v>41735</v>
       </c>
-      <c r="E23" s="36"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="36"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="38"/>
-      <c r="J23" s="35"/>
-      <c r="K23" s="23"/>
-      <c r="L23" s="35"/>
-      <c r="M23" s="36"/>
-      <c r="N23" s="19"/>
-    </row>
-    <row r="25" spans="1:14">
-      <c r="A25" s="13" t="s">
+      <c r="E18" s="36"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="38"/>
+      <c r="J18" s="35"/>
+      <c r="K18" s="23"/>
+      <c r="L18" s="35"/>
+      <c r="M18" s="36"/>
+      <c r="N18" s="19"/>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="A20" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="B25" s="13"/>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="85" t="s">
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="85" t="s">
         <v>41</v>
       </c>
-      <c r="F25" s="85"/>
-    </row>
-    <row r="26" spans="1:14">
-      <c r="A26" s="12" t="s">
+      <c r="F20" s="85"/>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="B26" s="12"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="86" t="s">
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="86" t="s">
         <v>42</v>
       </c>
-      <c r="F26" s="86"/>
-    </row>
-    <row r="27" spans="1:14">
-      <c r="A27" s="11" t="s">
+      <c r="F21" s="86"/>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="A22" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B27" s="11"/>
-      <c r="C27" s="11"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="87" t="s">
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="87" t="s">
         <v>38</v>
       </c>
-      <c r="F27" s="87"/>
-    </row>
-    <row r="28" spans="1:14">
-      <c r="A28" s="84" t="s">
+      <c r="F22" s="87"/>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="A23" s="84" t="s">
         <v>49</v>
       </c>
-      <c r="B28" s="84"/>
-      <c r="C28" s="84"/>
-      <c r="D28" s="84"/>
-      <c r="E28" s="84"/>
-      <c r="F28" s="84"/>
-    </row>
-    <row r="29" spans="1:14">
-      <c r="A29" s="83" t="s">
+      <c r="B23" s="84"/>
+      <c r="C23" s="84"/>
+      <c r="D23" s="84"/>
+      <c r="E23" s="84"/>
+      <c r="F23" s="84"/>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="A24" s="83" t="s">
         <v>61</v>
       </c>
-      <c r="B29" s="83"/>
-      <c r="C29" s="83"/>
-      <c r="D29" s="83"/>
-      <c r="E29" s="83"/>
-      <c r="F29" s="83"/>
+      <c r="B24" s="83"/>
+      <c r="C24" s="83"/>
+      <c r="D24" s="83"/>
+      <c r="E24" s="83"/>
+      <c r="F24" s="83"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="A28:F28"/>
-    <mergeCell ref="A29:F29"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="A23:F23"/>
+    <mergeCell ref="A24:F24"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>

<commit_message>
updated schedule for embedded
</commit_message>
<xml_diff>
--- a/Admin stuff/ganttChart copy.xlsx
+++ b/Admin stuff/ganttChart copy.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="95">
   <si>
     <t>Task</t>
   </si>
@@ -305,7 +305,23 @@
     <t>Testing and Integration</t>
   </si>
   <si>
-    <t>DC Auxilary Drivers</t>
+    <t>GroBot.h File</t>
+  </si>
+  <si>
+    <t>Channel Drivers</t>
+  </si>
+  <si>
+    <t>Http Request</t>
+  </si>
+  <si>
+    <t>DEMO
+4/29</t>
+  </si>
+  <si>
+    <t>Main.c:: event loop, init timers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testing </t>
   </si>
 </sst>
 </file>
@@ -476,7 +492,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="46">
+  <borders count="47">
     <border>
       <left/>
       <right/>
@@ -1043,8 +1059,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1058,8 +1083,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="132">
+  <cellXfs count="134">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1222,20 +1249,24 @@
     <xf numFmtId="0" fontId="0" fillId="17" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3885,10 +3916,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N24"/>
+  <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3937,7 +3968,9 @@
       <c r="L1" s="88" t="s">
         <v>81</v>
       </c>
-      <c r="M1" s="88"/>
+      <c r="M1" s="88" t="s">
+        <v>92</v>
+      </c>
       <c r="N1" s="88"/>
     </row>
     <row r="2" spans="1:14" ht="16" thickBot="1">
@@ -4114,13 +4147,13 @@
         <v>3</v>
       </c>
       <c r="D9" s="70">
-        <f t="shared" ref="D9:D18" si="1">B9+C9*7</f>
+        <f t="shared" ref="D9:D19" si="1">B9+C9*7</f>
         <v>41700</v>
       </c>
-      <c r="E9" s="41"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="46"/>
-      <c r="H9" s="55"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="30"/>
       <c r="I9" s="30"/>
       <c r="J9" s="14"/>
       <c r="K9" s="30"/>
@@ -4130,7 +4163,7 @@
     </row>
     <row r="10" spans="1:14" ht="16" thickBot="1">
       <c r="A10" s="22" t="s">
-        <v>13</v>
+        <v>90</v>
       </c>
       <c r="B10" s="70">
         <v>41673</v>
@@ -4142,10 +4175,9 @@
         <f t="shared" si="1"/>
         <v>41701</v>
       </c>
-      <c r="E10" s="45"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="47"/>
-      <c r="H10" s="56"/>
+      <c r="E10" s="42"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="15"/>
       <c r="I10" s="30"/>
       <c r="J10" s="14"/>
       <c r="K10" s="30"/>
@@ -4155,7 +4187,7 @@
     </row>
     <row r="11" spans="1:14" ht="16" thickBot="1">
       <c r="A11" s="22" t="s">
-        <v>15</v>
+        <v>93</v>
       </c>
       <c r="B11" s="70">
         <v>41686</v>
@@ -4169,10 +4201,9 @@
       </c>
       <c r="E11" s="41"/>
       <c r="F11" s="61"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="25"/>
-      <c r="I11" s="32"/>
-      <c r="J11" s="56"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="15"/>
       <c r="K11" s="30"/>
       <c r="L11" s="14"/>
       <c r="M11" s="30"/>
@@ -4180,240 +4211,254 @@
     </row>
     <row r="12" spans="1:14" ht="16" thickBot="1">
       <c r="A12" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="70">
-        <v>41700</v>
-      </c>
-      <c r="C12" s="77">
-        <v>3</v>
-      </c>
-      <c r="D12" s="70">
-        <f t="shared" si="1"/>
-        <v>41721</v>
-      </c>
-      <c r="E12" s="30"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="63"/>
-      <c r="I12" s="42"/>
-      <c r="J12" s="31"/>
-      <c r="K12" s="54"/>
+        <v>94</v>
+      </c>
+      <c r="B12" s="70"/>
+      <c r="C12" s="77"/>
+      <c r="D12" s="70"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="132"/>
+      <c r="H12" s="133"/>
+      <c r="I12" s="133"/>
+      <c r="J12" s="133"/>
+      <c r="K12" s="133"/>
       <c r="L12" s="14"/>
       <c r="M12" s="30"/>
       <c r="N12" s="15"/>
     </row>
     <row r="13" spans="1:14" ht="16" thickBot="1">
-      <c r="A13" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="B13" s="71">
-        <v>41679</v>
-      </c>
-      <c r="C13" s="78">
-        <v>4</v>
-      </c>
-      <c r="D13" s="71">
+      <c r="A13" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="B13" s="70">
+        <v>41700</v>
+      </c>
+      <c r="C13" s="77">
+        <v>3</v>
+      </c>
+      <c r="D13" s="70">
         <f t="shared" si="1"/>
-        <v>41707</v>
-      </c>
-      <c r="E13" s="124"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="33"/>
-      <c r="I13" s="33"/>
-      <c r="J13" s="57"/>
-      <c r="K13" s="30"/>
+        <v>41721</v>
+      </c>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="28"/>
       <c r="L13" s="14"/>
       <c r="M13" s="30"/>
       <c r="N13" s="15"/>
     </row>
     <row r="14" spans="1:14" ht="16" thickBot="1">
       <c r="A14" s="21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B14" s="71">
-        <v>41686</v>
+        <v>41679</v>
       </c>
       <c r="C14" s="78">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D14" s="71">
         <f t="shared" si="1"/>
         <v>41707</v>
       </c>
-      <c r="E14" s="59"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="125"/>
-      <c r="H14" s="82"/>
-      <c r="I14" s="57"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="30"/>
+      <c r="E14" s="124"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="33"/>
+      <c r="I14" s="33"/>
+      <c r="J14" s="57"/>
+      <c r="K14" s="57"/>
       <c r="L14" s="14"/>
       <c r="M14" s="30"/>
       <c r="N14" s="15"/>
     </row>
     <row r="15" spans="1:14" ht="16" thickBot="1">
       <c r="A15" s="21" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="B15" s="71">
-        <v>41707</v>
+        <v>41686</v>
       </c>
       <c r="C15" s="78">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D15" s="71">
         <f t="shared" si="1"/>
-        <v>41714</v>
-      </c>
-      <c r="E15" s="124"/>
-      <c r="F15" s="126"/>
-      <c r="G15" s="127"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="58"/>
-      <c r="J15" s="30"/>
-      <c r="K15" s="15"/>
+        <v>41707</v>
+      </c>
+      <c r="E15" s="59"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="125"/>
+      <c r="H15" s="82"/>
+      <c r="I15" s="57"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="30"/>
       <c r="L15" s="14"/>
       <c r="M15" s="30"/>
       <c r="N15" s="15"/>
     </row>
     <row r="16" spans="1:14" ht="16" thickBot="1">
-      <c r="A16" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="B16" s="66">
-        <v>41673</v>
-      </c>
-      <c r="C16" s="79">
-        <v>4</v>
-      </c>
-      <c r="D16" s="66">
+      <c r="A16" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="71">
+        <v>41707</v>
+      </c>
+      <c r="C16" s="78">
+        <v>1</v>
+      </c>
+      <c r="D16" s="71">
         <f t="shared" si="1"/>
-        <v>41701</v>
-      </c>
-      <c r="E16" s="128"/>
-      <c r="F16" s="35"/>
-      <c r="G16" s="129"/>
-      <c r="H16" s="60"/>
-      <c r="I16" s="34"/>
-      <c r="J16" s="16"/>
-      <c r="K16" s="30"/>
+        <v>41714</v>
+      </c>
+      <c r="E16" s="124"/>
+      <c r="F16" s="126"/>
+      <c r="G16" s="127"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="58"/>
+      <c r="J16" s="30"/>
+      <c r="K16" s="15"/>
       <c r="L16" s="14"/>
       <c r="M16" s="30"/>
       <c r="N16" s="15"/>
     </row>
     <row r="17" spans="1:14" ht="16" thickBot="1">
       <c r="A17" s="20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B17" s="66">
-        <v>41693</v>
+        <v>41673</v>
       </c>
       <c r="C17" s="79">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D17" s="66">
         <f t="shared" si="1"/>
-        <v>41714</v>
-      </c>
-      <c r="E17" s="30"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="130"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="131"/>
-      <c r="K17" s="34"/>
+        <v>41701</v>
+      </c>
+      <c r="E17" s="128"/>
+      <c r="F17" s="35"/>
+      <c r="G17" s="129"/>
+      <c r="H17" s="60"/>
+      <c r="I17" s="34"/>
+      <c r="J17" s="16"/>
+      <c r="K17" s="30"/>
       <c r="L17" s="14"/>
       <c r="M17" s="30"/>
       <c r="N17" s="15"/>
     </row>
     <row r="18" spans="1:14" ht="16" thickBot="1">
       <c r="A18" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="B18" s="72">
-        <v>41714</v>
-      </c>
-      <c r="C18" s="80">
+        <v>47</v>
+      </c>
+      <c r="B18" s="66">
+        <v>41693</v>
+      </c>
+      <c r="C18" s="79">
         <v>3</v>
       </c>
       <c r="D18" s="66">
         <f t="shared" si="1"/>
+        <v>41714</v>
+      </c>
+      <c r="E18" s="30"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="130"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="131"/>
+      <c r="K18" s="34"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="30"/>
+      <c r="N18" s="15"/>
+    </row>
+    <row r="19" spans="1:14" ht="16" thickBot="1">
+      <c r="A19" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" s="72">
+        <v>41714</v>
+      </c>
+      <c r="C19" s="80">
+        <v>3</v>
+      </c>
+      <c r="D19" s="66">
+        <f t="shared" si="1"/>
         <v>41735</v>
       </c>
-      <c r="E18" s="36"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="38"/>
-      <c r="J18" s="35"/>
-      <c r="K18" s="23"/>
-      <c r="L18" s="35"/>
-      <c r="M18" s="36"/>
-      <c r="N18" s="19"/>
-    </row>
-    <row r="20" spans="1:14">
-      <c r="A20" s="13" t="s">
+      <c r="E19" s="36"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="36"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="38"/>
+      <c r="J19" s="35"/>
+      <c r="K19" s="23"/>
+      <c r="L19" s="35"/>
+      <c r="M19" s="36"/>
+      <c r="N19" s="19"/>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="85" t="s">
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="85" t="s">
         <v>41</v>
       </c>
-      <c r="F20" s="85"/>
-    </row>
-    <row r="21" spans="1:14">
-      <c r="A21" s="12" t="s">
+      <c r="F21" s="85"/>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="A22" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="86" t="s">
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="86" t="s">
         <v>42</v>
       </c>
-      <c r="F21" s="86"/>
-    </row>
-    <row r="22" spans="1:14">
-      <c r="A22" s="11" t="s">
+      <c r="F22" s="86"/>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="A23" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B22" s="11"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="87" t="s">
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="87" t="s">
         <v>38</v>
       </c>
-      <c r="F22" s="87"/>
-    </row>
-    <row r="23" spans="1:14">
-      <c r="A23" s="84" t="s">
+      <c r="F23" s="87"/>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="A24" s="84" t="s">
         <v>49</v>
       </c>
-      <c r="B23" s="84"/>
-      <c r="C23" s="84"/>
-      <c r="D23" s="84"/>
-      <c r="E23" s="84"/>
-      <c r="F23" s="84"/>
-    </row>
-    <row r="24" spans="1:14">
-      <c r="A24" s="83" t="s">
+      <c r="B24" s="84"/>
+      <c r="C24" s="84"/>
+      <c r="D24" s="84"/>
+      <c r="E24" s="84"/>
+      <c r="F24" s="84"/>
+    </row>
+    <row r="25" spans="1:14">
+      <c r="A25" s="83" t="s">
         <v>61</v>
       </c>
-      <c r="B24" s="83"/>
-      <c r="C24" s="83"/>
-      <c r="D24" s="83"/>
-      <c r="E24" s="83"/>
-      <c r="F24" s="83"/>
+      <c r="B25" s="83"/>
+      <c r="C25" s="83"/>
+      <c r="D25" s="83"/>
+      <c r="E25" s="83"/>
+      <c r="F25" s="83"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="E20:F20"/>
     <mergeCell ref="E21:F21"/>
     <mergeCell ref="E22:F22"/>
-    <mergeCell ref="A23:F23"/>
+    <mergeCell ref="E23:F23"/>
     <mergeCell ref="A24:F24"/>
+    <mergeCell ref="A25:F25"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>

<commit_message>
added testing for embedded, cleaned up formatting
</commit_message>
<xml_diff>
--- a/Admin stuff/ganttChart copy.xlsx
+++ b/Admin stuff/ganttChart copy.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="96">
   <si>
     <t>Task</t>
   </si>
@@ -321,7 +321,10 @@
     <t>Main.c:: event loop, init timers</t>
   </si>
   <si>
-    <t xml:space="preserve">Testing </t>
+    <t>Testing with Website</t>
+  </si>
+  <si>
+    <t>Tesing with Hardware</t>
   </si>
 </sst>
 </file>
@@ -1060,11 +1063,13 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -1086,7 +1091,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="134">
+  <cellXfs count="137">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1249,8 +1254,11 @@
     <xf numFmtId="0" fontId="0" fillId="17" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -3916,10 +3924,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N25"/>
+  <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4147,11 +4155,11 @@
         <v>3</v>
       </c>
       <c r="D9" s="70">
-        <f t="shared" ref="D9:D19" si="1">B9+C9*7</f>
+        <f t="shared" ref="D9:D20" si="1">B9+C9*7</f>
         <v>41700</v>
       </c>
-      <c r="E9" s="42"/>
-      <c r="F9" s="30"/>
+      <c r="E9" s="132"/>
+      <c r="F9" s="15"/>
       <c r="G9" s="14"/>
       <c r="H9" s="30"/>
       <c r="I9" s="30"/>
@@ -4163,47 +4171,41 @@
     </row>
     <row r="10" spans="1:14" ht="16" thickBot="1">
       <c r="A10" s="22" t="s">
-        <v>90</v>
-      </c>
-      <c r="B10" s="70">
-        <v>41673</v>
-      </c>
-      <c r="C10" s="77">
-        <v>4</v>
-      </c>
-      <c r="D10" s="70">
-        <f t="shared" si="1"/>
-        <v>41701</v>
-      </c>
-      <c r="E10" s="42"/>
+        <v>95</v>
+      </c>
+      <c r="B10" s="70"/>
+      <c r="C10" s="77"/>
+      <c r="D10" s="70"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="30"/>
       <c r="G10" s="30"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="30"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="30"/>
+      <c r="H10" s="133"/>
+      <c r="I10" s="42"/>
+      <c r="J10" s="42"/>
+      <c r="K10" s="42"/>
       <c r="L10" s="14"/>
       <c r="M10" s="30"/>
       <c r="N10" s="15"/>
     </row>
     <row r="11" spans="1:14" ht="16" thickBot="1">
       <c r="A11" s="22" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B11" s="70">
-        <v>41686</v>
+        <v>41673</v>
       </c>
       <c r="C11" s="77">
         <v>4</v>
       </c>
       <c r="D11" s="70">
         <f t="shared" si="1"/>
-        <v>41714</v>
-      </c>
-      <c r="E11" s="41"/>
-      <c r="F11" s="61"/>
-      <c r="H11" s="28"/>
+        <v>41701</v>
+      </c>
+      <c r="E11" s="132"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="15"/>
       <c r="I11" s="30"/>
-      <c r="J11" s="15"/>
+      <c r="J11" s="14"/>
       <c r="K11" s="30"/>
       <c r="L11" s="14"/>
       <c r="M11" s="30"/>
@@ -4211,254 +4213,278 @@
     </row>
     <row r="12" spans="1:14" ht="16" thickBot="1">
       <c r="A12" s="22" t="s">
-        <v>94</v>
-      </c>
-      <c r="B12" s="70"/>
-      <c r="C12" s="77"/>
-      <c r="D12" s="70"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="132"/>
-      <c r="H12" s="133"/>
-      <c r="I12" s="133"/>
-      <c r="J12" s="133"/>
-      <c r="K12" s="133"/>
+        <v>93</v>
+      </c>
+      <c r="B12" s="70">
+        <v>41686</v>
+      </c>
+      <c r="C12" s="77">
+        <v>4</v>
+      </c>
+      <c r="D12" s="70">
+        <f t="shared" si="1"/>
+        <v>41714</v>
+      </c>
+      <c r="E12" s="41"/>
+      <c r="F12" s="30"/>
+      <c r="H12" s="135"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="30"/>
       <c r="L12" s="14"/>
       <c r="M12" s="30"/>
       <c r="N12" s="15"/>
     </row>
     <row r="13" spans="1:14" ht="16" thickBot="1">
       <c r="A13" s="22" t="s">
-        <v>91</v>
-      </c>
-      <c r="B13" s="70">
-        <v>41700</v>
-      </c>
-      <c r="C13" s="77">
-        <v>3</v>
-      </c>
-      <c r="D13" s="70">
-        <f t="shared" si="1"/>
-        <v>41721</v>
-      </c>
-      <c r="E13" s="28"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="28"/>
+        <v>94</v>
+      </c>
+      <c r="B13" s="70"/>
+      <c r="C13" s="77"/>
+      <c r="D13" s="70"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="136"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="32"/>
+      <c r="J13" s="32"/>
+      <c r="K13" s="134"/>
       <c r="L13" s="14"/>
       <c r="M13" s="30"/>
       <c r="N13" s="15"/>
     </row>
     <row r="14" spans="1:14" ht="16" thickBot="1">
-      <c r="A14" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="B14" s="71">
-        <v>41679</v>
-      </c>
-      <c r="C14" s="78">
-        <v>4</v>
-      </c>
-      <c r="D14" s="71">
+      <c r="A14" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="B14" s="70">
+        <v>41700</v>
+      </c>
+      <c r="C14" s="77">
+        <v>3</v>
+      </c>
+      <c r="D14" s="70">
         <f t="shared" si="1"/>
-        <v>41707</v>
-      </c>
-      <c r="E14" s="124"/>
-      <c r="F14" s="33"/>
-      <c r="G14" s="33"/>
-      <c r="H14" s="33"/>
-      <c r="I14" s="33"/>
-      <c r="J14" s="57"/>
-      <c r="K14" s="57"/>
+        <v>41721</v>
+      </c>
+      <c r="E14" s="28"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="134"/>
       <c r="L14" s="14"/>
       <c r="M14" s="30"/>
       <c r="N14" s="15"/>
     </row>
     <row r="15" spans="1:14" ht="16" thickBot="1">
       <c r="A15" s="21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B15" s="71">
-        <v>41686</v>
+        <v>41679</v>
       </c>
       <c r="C15" s="78">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D15" s="71">
         <f t="shared" si="1"/>
         <v>41707</v>
       </c>
-      <c r="E15" s="59"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="125"/>
-      <c r="H15" s="82"/>
-      <c r="I15" s="57"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="30"/>
+      <c r="E15" s="124"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="33"/>
+      <c r="H15" s="33"/>
+      <c r="I15" s="33"/>
+      <c r="J15" s="57"/>
+      <c r="K15" s="57"/>
       <c r="L15" s="14"/>
       <c r="M15" s="30"/>
       <c r="N15" s="15"/>
     </row>
     <row r="16" spans="1:14" ht="16" thickBot="1">
       <c r="A16" s="21" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="B16" s="71">
-        <v>41707</v>
+        <v>41686</v>
       </c>
       <c r="C16" s="78">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D16" s="71">
         <f t="shared" si="1"/>
-        <v>41714</v>
-      </c>
-      <c r="E16" s="124"/>
-      <c r="F16" s="126"/>
-      <c r="G16" s="127"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="58"/>
-      <c r="J16" s="30"/>
-      <c r="K16" s="15"/>
+        <v>41707</v>
+      </c>
+      <c r="E16" s="59"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="125"/>
+      <c r="H16" s="82"/>
+      <c r="I16" s="57"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="30"/>
       <c r="L16" s="14"/>
       <c r="M16" s="30"/>
       <c r="N16" s="15"/>
     </row>
     <row r="17" spans="1:14" ht="16" thickBot="1">
-      <c r="A17" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="B17" s="66">
-        <v>41673</v>
-      </c>
-      <c r="C17" s="79">
-        <v>4</v>
-      </c>
-      <c r="D17" s="66">
+      <c r="A17" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="71">
+        <v>41707</v>
+      </c>
+      <c r="C17" s="78">
+        <v>1</v>
+      </c>
+      <c r="D17" s="71">
         <f t="shared" si="1"/>
-        <v>41701</v>
-      </c>
-      <c r="E17" s="128"/>
-      <c r="F17" s="35"/>
-      <c r="G17" s="129"/>
-      <c r="H17" s="60"/>
-      <c r="I17" s="34"/>
-      <c r="J17" s="16"/>
-      <c r="K17" s="30"/>
+        <v>41714</v>
+      </c>
+      <c r="E17" s="124"/>
+      <c r="F17" s="126"/>
+      <c r="G17" s="127"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="58"/>
+      <c r="J17" s="30"/>
+      <c r="K17" s="15"/>
       <c r="L17" s="14"/>
       <c r="M17" s="30"/>
       <c r="N17" s="15"/>
     </row>
     <row r="18" spans="1:14" ht="16" thickBot="1">
       <c r="A18" s="20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B18" s="66">
-        <v>41693</v>
+        <v>41673</v>
       </c>
       <c r="C18" s="79">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D18" s="66">
         <f t="shared" si="1"/>
-        <v>41714</v>
-      </c>
-      <c r="E18" s="30"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="130"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="131"/>
-      <c r="K18" s="34"/>
+        <v>41701</v>
+      </c>
+      <c r="E18" s="128"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="129"/>
+      <c r="H18" s="60"/>
+      <c r="I18" s="34"/>
+      <c r="J18" s="16"/>
+      <c r="K18" s="30"/>
       <c r="L18" s="14"/>
       <c r="M18" s="30"/>
       <c r="N18" s="15"/>
     </row>
     <row r="19" spans="1:14" ht="16" thickBot="1">
       <c r="A19" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="B19" s="72">
-        <v>41714</v>
-      </c>
-      <c r="C19" s="80">
+        <v>47</v>
+      </c>
+      <c r="B19" s="66">
+        <v>41693</v>
+      </c>
+      <c r="C19" s="79">
         <v>3</v>
       </c>
       <c r="D19" s="66">
         <f t="shared" si="1"/>
+        <v>41714</v>
+      </c>
+      <c r="E19" s="30"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="130"/>
+      <c r="H19" s="35"/>
+      <c r="I19" s="131"/>
+      <c r="K19" s="34"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="30"/>
+      <c r="N19" s="15"/>
+    </row>
+    <row r="20" spans="1:14" ht="16" thickBot="1">
+      <c r="A20" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" s="72">
+        <v>41714</v>
+      </c>
+      <c r="C20" s="80">
+        <v>3</v>
+      </c>
+      <c r="D20" s="66">
+        <f t="shared" si="1"/>
         <v>41735</v>
       </c>
-      <c r="E19" s="36"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="36"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="38"/>
-      <c r="J19" s="35"/>
-      <c r="K19" s="23"/>
-      <c r="L19" s="35"/>
-      <c r="M19" s="36"/>
-      <c r="N19" s="19"/>
-    </row>
-    <row r="21" spans="1:14">
-      <c r="A21" s="13" t="s">
+      <c r="E20" s="36"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="36"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="38"/>
+      <c r="J20" s="35"/>
+      <c r="K20" s="23"/>
+      <c r="L20" s="35"/>
+      <c r="M20" s="36"/>
+      <c r="N20" s="19"/>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="A22" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="85" t="s">
+      <c r="B22" s="13"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="85" t="s">
         <v>41</v>
       </c>
-      <c r="F21" s="85"/>
-    </row>
-    <row r="22" spans="1:14">
-      <c r="A22" s="12" t="s">
+      <c r="F22" s="85"/>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="A23" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="12"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="86" t="s">
+      <c r="B23" s="12"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="86" t="s">
         <v>42</v>
       </c>
-      <c r="F22" s="86"/>
-    </row>
-    <row r="23" spans="1:14">
-      <c r="A23" s="11" t="s">
+      <c r="F23" s="86"/>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="A24" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="11"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="87" t="s">
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="87" t="s">
         <v>38</v>
       </c>
-      <c r="F23" s="87"/>
-    </row>
-    <row r="24" spans="1:14">
-      <c r="A24" s="84" t="s">
+      <c r="F24" s="87"/>
+    </row>
+    <row r="25" spans="1:14">
+      <c r="A25" s="84" t="s">
         <v>49</v>
       </c>
-      <c r="B24" s="84"/>
-      <c r="C24" s="84"/>
-      <c r="D24" s="84"/>
-      <c r="E24" s="84"/>
-      <c r="F24" s="84"/>
-    </row>
-    <row r="25" spans="1:14">
-      <c r="A25" s="83" t="s">
+      <c r="B25" s="84"/>
+      <c r="C25" s="84"/>
+      <c r="D25" s="84"/>
+      <c r="E25" s="84"/>
+      <c r="F25" s="84"/>
+    </row>
+    <row r="26" spans="1:14">
+      <c r="A26" s="83" t="s">
         <v>61</v>
       </c>
-      <c r="B25" s="83"/>
-      <c r="C25" s="83"/>
-      <c r="D25" s="83"/>
-      <c r="E25" s="83"/>
-      <c r="F25" s="83"/>
+      <c r="B26" s="83"/>
+      <c r="C26" s="83"/>
+      <c r="D26" s="83"/>
+      <c r="E26" s="83"/>
+      <c r="F26" s="83"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="E21:F21"/>
     <mergeCell ref="E22:F22"/>
     <mergeCell ref="E23:F23"/>
-    <mergeCell ref="A24:F24"/>
+    <mergeCell ref="E24:F24"/>
     <mergeCell ref="A25:F25"/>
+    <mergeCell ref="A26:F26"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>